<commit_message>
Added missing dates to change log
</commit_message>
<xml_diff>
--- a/documents/Change Log and Tests.xlsx
+++ b/documents/Change Log and Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\uniform-distribution-system\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5791E4FA-8538-4969-B197-3EB1B36B3B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE32251-5693-4197-84C0-0A1C2DBB1186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{75C8EF5A-735B-4C2E-9ED6-E549F9606222}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{75C8EF5A-735B-4C2E-9ED6-E549F9606222}"/>
   </bookViews>
   <sheets>
     <sheet name="Change Log" sheetId="11" r:id="rId1"/>
@@ -3345,7 +3345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3591,261 +3591,225 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3946,10 +3910,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4296,8 +4256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF10BFD-D0AE-4987-B6E5-86284210D0DF}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4764,7 +4724,9 @@
       <c r="D27" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="E27" s="10"/>
+      <c r="E27" s="10">
+        <v>45759</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
@@ -4779,7 +4741,9 @@
       <c r="D28" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="E28" s="10"/>
+      <c r="E28" s="10">
+        <v>45759</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
@@ -4794,7 +4758,9 @@
       <c r="D29" s="5" t="s">
         <v>805</v>
       </c>
-      <c r="E29" s="10"/>
+      <c r="E29" s="10">
+        <v>45759</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
@@ -4947,10 +4913,10 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="129" t="s">
         <v>68</v>
       </c>
       <c r="C2" s="60" t="s">
@@ -4978,8 +4944,8 @@
       <c r="K2" s="65"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="88"/>
-      <c r="B3" s="91"/>
+      <c r="A3" s="115"/>
+      <c r="B3" s="118"/>
       <c r="C3" s="34" t="s">
         <v>35</v>
       </c>
@@ -5005,8 +4971,8 @@
       <c r="K3" s="38"/>
     </row>
     <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="88"/>
-      <c r="B4" s="91"/>
+      <c r="A4" s="115"/>
+      <c r="B4" s="118"/>
       <c r="C4" s="34" t="s">
         <v>47</v>
       </c>
@@ -5032,8 +4998,8 @@
       <c r="K4" s="38"/>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="88"/>
-      <c r="B5" s="91"/>
+      <c r="A5" s="115"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="34" t="s">
         <v>48</v>
       </c>
@@ -5059,8 +5025,8 @@
       <c r="K5" s="38"/>
     </row>
     <row r="6" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="88"/>
-      <c r="B6" s="91"/>
+      <c r="A6" s="115"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="34" t="s">
         <v>49</v>
       </c>
@@ -5086,8 +5052,8 @@
       <c r="K6" s="38"/>
     </row>
     <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="88"/>
-      <c r="B7" s="91"/>
+      <c r="A7" s="115"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="34" t="s">
         <v>50</v>
       </c>
@@ -5113,8 +5079,8 @@
       <c r="K7" s="38"/>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="88"/>
-      <c r="B8" s="91"/>
+      <c r="A8" s="115"/>
+      <c r="B8" s="118"/>
       <c r="C8" s="34" t="s">
         <v>51</v>
       </c>
@@ -5142,8 +5108,8 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="89"/>
-      <c r="B9" s="92"/>
+      <c r="A9" s="116"/>
+      <c r="B9" s="119"/>
       <c r="C9" s="34" t="s">
         <v>52</v>
       </c>
@@ -5171,10 +5137,10 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="96" t="s">
+      <c r="B10" s="123" t="s">
         <v>71</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -5202,8 +5168,8 @@
       <c r="K10" s="52"/>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="94"/>
-      <c r="B11" s="97"/>
+      <c r="A11" s="121"/>
+      <c r="B11" s="124"/>
       <c r="C11" s="47" t="s">
         <v>54</v>
       </c>
@@ -5229,8 +5195,8 @@
       <c r="K11" s="52"/>
     </row>
     <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="94"/>
-      <c r="B12" s="97"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="124"/>
       <c r="C12" s="47" t="s">
         <v>55</v>
       </c>
@@ -5256,8 +5222,8 @@
       <c r="K12" s="52"/>
     </row>
     <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="94"/>
-      <c r="B13" s="97"/>
+      <c r="A13" s="121"/>
+      <c r="B13" s="124"/>
       <c r="C13" s="47" t="s">
         <v>56</v>
       </c>
@@ -5283,8 +5249,8 @@
       <c r="K13" s="52"/>
     </row>
     <row r="14" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="94"/>
-      <c r="B14" s="97"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="124"/>
       <c r="C14" s="47" t="s">
         <v>57</v>
       </c>
@@ -5310,8 +5276,8 @@
       <c r="K14" s="52"/>
     </row>
     <row r="15" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="95"/>
-      <c r="B15" s="98"/>
+      <c r="A15" s="127"/>
+      <c r="B15" s="126"/>
       <c r="C15" s="47" t="s">
         <v>58</v>
       </c>
@@ -5337,10 +5303,10 @@
       <c r="K15" s="52"/>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="99" t="s">
+      <c r="A16" s="114" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="100" t="s">
+      <c r="B16" s="117" t="s">
         <v>139</v>
       </c>
       <c r="C16" s="34" t="s">
@@ -5368,8 +5334,8 @@
       <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="88"/>
-      <c r="B17" s="91"/>
+      <c r="A17" s="115"/>
+      <c r="B17" s="118"/>
       <c r="C17" s="34" t="s">
         <v>73</v>
       </c>
@@ -5395,8 +5361,8 @@
       <c r="K17" s="38"/>
     </row>
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="88"/>
-      <c r="B18" s="91"/>
+      <c r="A18" s="115"/>
+      <c r="B18" s="118"/>
       <c r="C18" s="34" t="s">
         <v>74</v>
       </c>
@@ -5422,8 +5388,8 @@
       <c r="K18" s="38"/>
     </row>
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="88"/>
-      <c r="B19" s="91"/>
+      <c r="A19" s="115"/>
+      <c r="B19" s="118"/>
       <c r="C19" s="34" t="s">
         <v>75</v>
       </c>
@@ -5449,8 +5415,8 @@
       <c r="K19" s="38"/>
     </row>
     <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
-      <c r="B20" s="91"/>
+      <c r="A20" s="115"/>
+      <c r="B20" s="118"/>
       <c r="C20" s="34" t="s">
         <v>76</v>
       </c>
@@ -5476,8 +5442,8 @@
       <c r="K20" s="38"/>
     </row>
     <row r="21" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="88"/>
-      <c r="B21" s="91"/>
+      <c r="A21" s="115"/>
+      <c r="B21" s="118"/>
       <c r="C21" s="34" t="s">
         <v>77</v>
       </c>
@@ -5503,8 +5469,8 @@
       <c r="K21" s="38"/>
     </row>
     <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="88"/>
-      <c r="B22" s="91"/>
+      <c r="A22" s="115"/>
+      <c r="B22" s="118"/>
       <c r="C22" s="34" t="s">
         <v>78</v>
       </c>
@@ -5530,8 +5496,8 @@
       <c r="K22" s="38"/>
     </row>
     <row r="23" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="89"/>
-      <c r="B23" s="92"/>
+      <c r="A23" s="116"/>
+      <c r="B23" s="119"/>
       <c r="C23" s="34" t="s">
         <v>79</v>
       </c>
@@ -5557,10 +5523,10 @@
       <c r="K23" s="38"/>
     </row>
     <row r="24" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="93" t="s">
+      <c r="A24" s="120" t="s">
         <v>80</v>
       </c>
-      <c r="B24" s="96" t="s">
+      <c r="B24" s="123" t="s">
         <v>140</v>
       </c>
       <c r="C24" s="47" t="s">
@@ -5588,8 +5554,8 @@
       <c r="K24" s="52"/>
     </row>
     <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="94"/>
-      <c r="B25" s="97"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="124"/>
       <c r="C25" s="47" t="s">
         <v>82</v>
       </c>
@@ -5615,8 +5581,8 @@
       <c r="K25" s="52"/>
     </row>
     <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="94"/>
-      <c r="B26" s="97"/>
+      <c r="A26" s="121"/>
+      <c r="B26" s="124"/>
       <c r="C26" s="47" t="s">
         <v>83</v>
       </c>
@@ -5642,8 +5608,8 @@
       <c r="K26" s="52"/>
     </row>
     <row r="27" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="94"/>
-      <c r="B27" s="97"/>
+      <c r="A27" s="121"/>
+      <c r="B27" s="124"/>
       <c r="C27" s="47" t="s">
         <v>84</v>
       </c>
@@ -5669,8 +5635,8 @@
       <c r="K27" s="52"/>
     </row>
     <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="94"/>
-      <c r="B28" s="97"/>
+      <c r="A28" s="121"/>
+      <c r="B28" s="124"/>
       <c r="C28" s="47" t="s">
         <v>85</v>
       </c>
@@ -5696,8 +5662,8 @@
       <c r="K28" s="52"/>
     </row>
     <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="95"/>
-      <c r="B29" s="98"/>
+      <c r="A29" s="127"/>
+      <c r="B29" s="126"/>
       <c r="C29" s="47" t="s">
         <v>86</v>
       </c>
@@ -5723,10 +5689,10 @@
       <c r="K29" s="52"/>
     </row>
     <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="99" t="s">
+      <c r="A30" s="114" t="s">
         <v>396</v>
       </c>
-      <c r="B30" s="100" t="s">
+      <c r="B30" s="117" t="s">
         <v>406</v>
       </c>
       <c r="C30" s="34" t="s">
@@ -5754,8 +5720,8 @@
       <c r="K30" s="38"/>
     </row>
     <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="88"/>
-      <c r="B31" s="91"/>
+      <c r="A31" s="115"/>
+      <c r="B31" s="118"/>
       <c r="C31" s="34" t="s">
         <v>398</v>
       </c>
@@ -5781,8 +5747,8 @@
       <c r="K31" s="38"/>
     </row>
     <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="88"/>
-      <c r="B32" s="91"/>
+      <c r="A32" s="115"/>
+      <c r="B32" s="118"/>
       <c r="C32" s="34" t="s">
         <v>399</v>
       </c>
@@ -5808,8 +5774,8 @@
       <c r="K32" s="38"/>
     </row>
     <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="88"/>
-      <c r="B33" s="91"/>
+      <c r="A33" s="115"/>
+      <c r="B33" s="118"/>
       <c r="C33" s="34" t="s">
         <v>400</v>
       </c>
@@ -5835,8 +5801,8 @@
       <c r="K33" s="38"/>
     </row>
     <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="88"/>
-      <c r="B34" s="91"/>
+      <c r="A34" s="115"/>
+      <c r="B34" s="118"/>
       <c r="C34" s="34" t="s">
         <v>401</v>
       </c>
@@ -5862,8 +5828,8 @@
       <c r="K34" s="38"/>
     </row>
     <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="88"/>
-      <c r="B35" s="91"/>
+      <c r="A35" s="115"/>
+      <c r="B35" s="118"/>
       <c r="C35" s="34" t="s">
         <v>402</v>
       </c>
@@ -5889,8 +5855,8 @@
       <c r="K35" s="38"/>
     </row>
     <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="88"/>
-      <c r="B36" s="91"/>
+      <c r="A36" s="115"/>
+      <c r="B36" s="118"/>
       <c r="C36" s="34" t="s">
         <v>403</v>
       </c>
@@ -5916,8 +5882,8 @@
       <c r="K36" s="38"/>
     </row>
     <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="89"/>
-      <c r="B37" s="92"/>
+      <c r="A37" s="116"/>
+      <c r="B37" s="119"/>
       <c r="C37" s="34" t="s">
         <v>404</v>
       </c>
@@ -5943,10 +5909,10 @@
       <c r="K37" s="38"/>
     </row>
     <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="93" t="s">
+      <c r="A38" s="120" t="s">
         <v>407</v>
       </c>
-      <c r="B38" s="96" t="s">
+      <c r="B38" s="123" t="s">
         <v>405</v>
       </c>
       <c r="C38" s="47" t="s">
@@ -5974,8 +5940,8 @@
       <c r="K38" s="52"/>
     </row>
     <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="94"/>
-      <c r="B39" s="97"/>
+      <c r="A39" s="121"/>
+      <c r="B39" s="124"/>
       <c r="C39" s="47" t="s">
         <v>409</v>
       </c>
@@ -6001,8 +5967,8 @@
       <c r="K39" s="52"/>
     </row>
     <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="94"/>
-      <c r="B40" s="97"/>
+      <c r="A40" s="121"/>
+      <c r="B40" s="124"/>
       <c r="C40" s="47" t="s">
         <v>410</v>
       </c>
@@ -6028,8 +5994,8 @@
       <c r="K40" s="52"/>
     </row>
     <row r="41" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="94"/>
-      <c r="B41" s="97"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="124"/>
       <c r="C41" s="47" t="s">
         <v>411</v>
       </c>
@@ -6055,8 +6021,8 @@
       <c r="K41" s="52"/>
     </row>
     <row r="42" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="94"/>
-      <c r="B42" s="97"/>
+      <c r="A42" s="121"/>
+      <c r="B42" s="124"/>
       <c r="C42" s="47" t="s">
         <v>412</v>
       </c>
@@ -6082,8 +6048,8 @@
       <c r="K42" s="52"/>
     </row>
     <row r="43" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="101"/>
-      <c r="B43" s="102"/>
+      <c r="A43" s="122"/>
+      <c r="B43" s="125"/>
       <c r="C43" s="54" t="s">
         <v>413</v>
       </c>
@@ -6188,18 +6154,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="A16:A23"/>
+    <mergeCell ref="B16:B23"/>
     <mergeCell ref="A30:A37"/>
     <mergeCell ref="B30:B37"/>
     <mergeCell ref="A38:A43"/>
     <mergeCell ref="B38:B43"/>
     <mergeCell ref="B24:B29"/>
     <mergeCell ref="A24:A29"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="A16:A23"/>
-    <mergeCell ref="B16:B23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="H2:H43">
@@ -6278,10 +6244,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="128" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="129" t="s">
         <v>90</v>
       </c>
       <c r="C2" s="18" t="s">
@@ -6316,8 +6282,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="89"/>
-      <c r="B3" s="92"/>
+      <c r="A3" s="116"/>
+      <c r="B3" s="119"/>
       <c r="C3" s="34" t="s">
         <v>104</v>
       </c>
@@ -6380,10 +6346,10 @@
       <c r="L4" s="52"/>
     </row>
     <row r="5" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="114" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="117" t="s">
         <v>108</v>
       </c>
       <c r="C5" s="34" t="s">
@@ -6418,8 +6384,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="89"/>
-      <c r="B6" s="92"/>
+      <c r="A6" s="116"/>
+      <c r="B6" s="119"/>
       <c r="C6" s="24" t="s">
         <v>118</v>
       </c>
@@ -6450,10 +6416,10 @@
       <c r="L6" s="28"/>
     </row>
     <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="120" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="123" t="s">
         <v>145</v>
       </c>
       <c r="C7" s="47" t="s">
@@ -6486,8 +6452,8 @@
       <c r="L7" s="52"/>
     </row>
     <row r="8" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="95"/>
-      <c r="B8" s="98"/>
+      <c r="A8" s="127"/>
+      <c r="B8" s="126"/>
       <c r="C8" s="47" t="s">
         <v>122</v>
       </c>
@@ -6550,10 +6516,10 @@
       <c r="L9" s="38"/>
     </row>
     <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="120" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="96" t="s">
+      <c r="B10" s="123" t="s">
         <v>134</v>
       </c>
       <c r="C10" s="47" t="s">
@@ -6586,8 +6552,8 @@
       <c r="L10" s="52"/>
     </row>
     <row r="11" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="95"/>
-      <c r="B11" s="98"/>
+      <c r="A11" s="127"/>
+      <c r="B11" s="126"/>
       <c r="C11" s="47" t="s">
         <v>128</v>
       </c>
@@ -6620,10 +6586,10 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="99" t="s">
+      <c r="A12" s="114" t="s">
         <v>146</v>
       </c>
-      <c r="B12" s="100" t="s">
+      <c r="B12" s="117" t="s">
         <v>149</v>
       </c>
       <c r="C12" s="24" t="s">
@@ -6656,8 +6622,8 @@
       <c r="L12" s="28"/>
     </row>
     <row r="13" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="89"/>
-      <c r="B13" s="92"/>
+      <c r="A13" s="116"/>
+      <c r="B13" s="119"/>
       <c r="C13" s="34" t="s">
         <v>148</v>
       </c>
@@ -6688,10 +6654,10 @@
       <c r="L13" s="38"/>
     </row>
     <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="120" t="s">
         <v>350</v>
       </c>
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="123" t="s">
         <v>360</v>
       </c>
       <c r="C14" s="47" t="s">
@@ -6724,8 +6690,8 @@
       <c r="L14" s="52"/>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="94"/>
-      <c r="B15" s="97"/>
+      <c r="A15" s="121"/>
+      <c r="B15" s="124"/>
       <c r="C15" s="47" t="s">
         <v>358</v>
       </c>
@@ -6758,8 +6724,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="95"/>
-      <c r="B16" s="98"/>
+      <c r="A16" s="127"/>
+      <c r="B16" s="126"/>
       <c r="C16" s="47" t="s">
         <v>359</v>
       </c>
@@ -6790,10 +6756,10 @@
       <c r="L16" s="52"/>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="99" t="s">
+      <c r="A17" s="114" t="s">
         <v>414</v>
       </c>
-      <c r="B17" s="100" t="s">
+      <c r="B17" s="117" t="s">
         <v>430</v>
       </c>
       <c r="C17" s="34" t="s">
@@ -6828,8 +6794,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="89"/>
-      <c r="B18" s="92"/>
+      <c r="A18" s="116"/>
+      <c r="B18" s="119"/>
       <c r="C18" s="24" t="s">
         <v>431</v>
       </c>
@@ -6858,10 +6824,10 @@
       <c r="L18" s="28"/>
     </row>
     <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="93" t="s">
+      <c r="A19" s="120" t="s">
         <v>417</v>
       </c>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="123" t="s">
         <v>435</v>
       </c>
       <c r="C19" s="47" t="s">
@@ -6892,8 +6858,8 @@
       <c r="L19" s="52"/>
     </row>
     <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="94"/>
-      <c r="B20" s="97"/>
+      <c r="A20" s="121"/>
+      <c r="B20" s="124"/>
       <c r="C20" s="47" t="s">
         <v>437</v>
       </c>
@@ -6924,8 +6890,8 @@
       <c r="L20" s="52"/>
     </row>
     <row r="21" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="95"/>
-      <c r="B21" s="98"/>
+      <c r="A21" s="127"/>
+      <c r="B21" s="126"/>
       <c r="C21" s="47" t="s">
         <v>438</v>
       </c>
@@ -6956,10 +6922,10 @@
       <c r="L21" s="52"/>
     </row>
     <row r="22" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="99" t="s">
+      <c r="A22" s="114" t="s">
         <v>451</v>
       </c>
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="117" t="s">
         <v>463</v>
       </c>
       <c r="C22" s="24" t="s">
@@ -6992,8 +6958,8 @@
       <c r="L22" s="28"/>
     </row>
     <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="88"/>
-      <c r="B23" s="91"/>
+      <c r="A23" s="115"/>
+      <c r="B23" s="118"/>
       <c r="C23" s="34" t="s">
         <v>459</v>
       </c>
@@ -7024,8 +6990,8 @@
       <c r="L23" s="38"/>
     </row>
     <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="89"/>
-      <c r="B24" s="92"/>
+      <c r="A24" s="116"/>
+      <c r="B24" s="119"/>
       <c r="C24" s="24" t="s">
         <v>460</v>
       </c>
@@ -7088,10 +7054,10 @@
       <c r="L25" s="52"/>
     </row>
     <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="99" t="s">
+      <c r="A26" s="114" t="s">
         <v>470</v>
       </c>
-      <c r="B26" s="100" t="s">
+      <c r="B26" s="117" t="s">
         <v>471</v>
       </c>
       <c r="C26" s="24" t="s">
@@ -7120,8 +7086,8 @@
       <c r="L26" s="28"/>
     </row>
     <row r="27" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="88"/>
-      <c r="B27" s="91"/>
+      <c r="A27" s="115"/>
+      <c r="B27" s="118"/>
       <c r="C27" s="34" t="s">
         <v>476</v>
       </c>
@@ -7148,8 +7114,8 @@
       <c r="L27" s="38"/>
     </row>
     <row r="28" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="88"/>
-      <c r="B28" s="91"/>
+      <c r="A28" s="115"/>
+      <c r="B28" s="118"/>
       <c r="C28" s="24" t="s">
         <v>477</v>
       </c>
@@ -7176,8 +7142,8 @@
       <c r="L28" s="28"/>
     </row>
     <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="89"/>
-      <c r="B29" s="92"/>
+      <c r="A29" s="116"/>
+      <c r="B29" s="119"/>
       <c r="C29" s="34" t="s">
         <v>478</v>
       </c>
@@ -7236,10 +7202,10 @@
       <c r="L30" s="52"/>
     </row>
     <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="99" t="s">
+      <c r="A31" s="114" t="s">
         <v>493</v>
       </c>
-      <c r="B31" s="100" t="s">
+      <c r="B31" s="117" t="s">
         <v>504</v>
       </c>
       <c r="C31" s="34" t="s">
@@ -7270,8 +7236,8 @@
       <c r="L31" s="38"/>
     </row>
     <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="89"/>
-      <c r="B32" s="92"/>
+      <c r="A32" s="116"/>
+      <c r="B32" s="119"/>
       <c r="C32" s="24" t="s">
         <v>495</v>
       </c>
@@ -7298,10 +7264,10 @@
       <c r="L32" s="28"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="93" t="s">
+      <c r="A33" s="120" t="s">
         <v>502</v>
       </c>
-      <c r="B33" s="96" t="s">
+      <c r="B33" s="123" t="s">
         <v>503</v>
       </c>
       <c r="C33" s="47" t="s">
@@ -7330,8 +7296,8 @@
       <c r="L33" s="52"/>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="95"/>
-      <c r="B34" s="98"/>
+      <c r="A34" s="127"/>
+      <c r="B34" s="126"/>
       <c r="C34" s="47" t="s">
         <v>510</v>
       </c>
@@ -7448,10 +7414,10 @@
       <c r="L37" s="38"/>
     </row>
     <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="93" t="s">
+      <c r="A38" s="120" t="s">
         <v>598</v>
       </c>
-      <c r="B38" s="96" t="s">
+      <c r="B38" s="123" t="s">
         <v>599</v>
       </c>
       <c r="C38" s="47" t="s">
@@ -7484,8 +7450,8 @@
       <c r="L38" s="52"/>
     </row>
     <row r="39" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="94"/>
-      <c r="B39" s="97"/>
+      <c r="A39" s="121"/>
+      <c r="B39" s="124"/>
       <c r="C39" s="47" t="s">
         <v>459</v>
       </c>
@@ -7516,8 +7482,8 @@
       <c r="L39" s="52"/>
     </row>
     <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="95"/>
-      <c r="B40" s="98"/>
+      <c r="A40" s="127"/>
+      <c r="B40" s="126"/>
       <c r="C40" s="47" t="s">
         <v>460</v>
       </c>
@@ -7548,10 +7514,10 @@
       <c r="L40" s="52"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="99" t="s">
+      <c r="A41" s="114" t="s">
         <v>604</v>
       </c>
-      <c r="B41" s="100" t="s">
+      <c r="B41" s="117" t="s">
         <v>606</v>
       </c>
       <c r="C41" s="34" t="s">
@@ -7580,8 +7546,8 @@
       <c r="L41" s="38"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="88"/>
-      <c r="B42" s="91"/>
+      <c r="A42" s="115"/>
+      <c r="B42" s="118"/>
       <c r="C42" s="24" t="s">
         <v>607</v>
       </c>
@@ -7610,8 +7576,8 @@
       <c r="L42" s="28"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="104"/>
-      <c r="B43" s="103"/>
+      <c r="A43" s="131"/>
+      <c r="B43" s="130"/>
       <c r="C43" s="40" t="s">
         <v>615</v>
       </c>
@@ -7717,6 +7683,24 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A22:A24"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="B41:B43"/>
@@ -7727,24 +7711,6 @@
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I2:I43">
@@ -7823,10 +7789,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="132" t="s">
         <v>536</v>
       </c>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="135" t="s">
         <v>529</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -7855,8 +7821,8 @@
       <c r="L2" s="72"/>
     </row>
     <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="108"/>
-      <c r="B3" s="111"/>
+      <c r="A3" s="133"/>
+      <c r="B3" s="136"/>
       <c r="C3" s="32" t="s">
         <v>569</v>
       </c>
@@ -7883,8 +7849,8 @@
       <c r="L3" s="79"/>
     </row>
     <row r="4" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="109"/>
-      <c r="B4" s="112"/>
+      <c r="A4" s="134"/>
+      <c r="B4" s="137"/>
       <c r="C4" s="23" t="s">
         <v>570</v>
       </c>
@@ -7977,10 +7943,10 @@
       <c r="L6" s="77"/>
     </row>
     <row r="7" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="138" t="s">
         <v>539</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="123" t="s">
         <v>532</v>
       </c>
       <c r="C7" s="47" t="s">
@@ -8011,8 +7977,8 @@
       <c r="L7" s="74"/>
     </row>
     <row r="8" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="117"/>
-      <c r="B8" s="97"/>
+      <c r="A8" s="139"/>
+      <c r="B8" s="124"/>
       <c r="C8" s="47" t="s">
         <v>585</v>
       </c>
@@ -8039,8 +8005,8 @@
       <c r="L8" s="74"/>
     </row>
     <row r="9" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A9" s="118"/>
-      <c r="B9" s="98"/>
+      <c r="A9" s="140"/>
+      <c r="B9" s="126"/>
       <c r="C9" s="47" t="s">
         <v>586</v>
       </c>
@@ -8067,10 +8033,10 @@
       <c r="L9" s="74"/>
     </row>
     <row r="10" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="141" t="s">
         <v>540</v>
       </c>
-      <c r="B10" s="110" t="s">
+      <c r="B10" s="142" t="s">
         <v>533</v>
       </c>
       <c r="C10" s="24" t="s">
@@ -8101,8 +8067,8 @@
       <c r="L10" s="77"/>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="109"/>
-      <c r="B11" s="112"/>
+      <c r="A11" s="134"/>
+      <c r="B11" s="137"/>
       <c r="C11" s="34" t="s">
         <v>587</v>
       </c>
@@ -8163,10 +8129,10 @@
       <c r="L12" s="74"/>
     </row>
     <row r="13" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="105" t="s">
+      <c r="A13" s="143" t="s">
         <v>542</v>
       </c>
-      <c r="B13" s="100" t="s">
+      <c r="B13" s="117" t="s">
         <v>535</v>
       </c>
       <c r="C13" s="34" t="s">
@@ -8195,8 +8161,8 @@
       <c r="L13" s="79"/>
     </row>
     <row r="14" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="106"/>
-      <c r="B14" s="92"/>
+      <c r="A14" s="144"/>
+      <c r="B14" s="119"/>
       <c r="C14" s="24" t="s">
         <v>557</v>
       </c>
@@ -8255,10 +8221,10 @@
       <c r="L15" s="74"/>
     </row>
     <row r="16" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A16" s="107" t="s">
+      <c r="A16" s="141" t="s">
         <v>621</v>
       </c>
-      <c r="B16" s="110" t="s">
+      <c r="B16" s="142" t="s">
         <v>532</v>
       </c>
       <c r="C16" s="24" t="s">
@@ -8289,8 +8255,8 @@
       <c r="L16" s="77"/>
     </row>
     <row r="17" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A17" s="108"/>
-      <c r="B17" s="111"/>
+      <c r="A17" s="133"/>
+      <c r="B17" s="136"/>
       <c r="C17" s="34" t="s">
         <v>623</v>
       </c>
@@ -8317,8 +8283,8 @@
       <c r="L17" s="79"/>
     </row>
     <row r="18" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" s="109"/>
-      <c r="B18" s="112"/>
+      <c r="A18" s="134"/>
+      <c r="B18" s="137"/>
       <c r="C18" s="24" t="s">
         <v>624</v>
       </c>
@@ -8345,10 +8311,10 @@
       <c r="L18" s="77"/>
     </row>
     <row r="19" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="113" t="s">
+      <c r="A19" s="138" t="s">
         <v>630</v>
       </c>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="123" t="s">
         <v>533</v>
       </c>
       <c r="C19" s="47" t="s">
@@ -8379,8 +8345,8 @@
       <c r="L19" s="74"/>
     </row>
     <row r="20" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="114"/>
-      <c r="B20" s="102"/>
+      <c r="A20" s="145"/>
+      <c r="B20" s="125"/>
       <c r="C20" s="54" t="s">
         <v>632</v>
       </c>
@@ -8791,18 +8757,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="I2:I20">
@@ -8822,7 +8788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9887801-C2EB-4E4A-A88F-D709B069AA5F}">
   <dimension ref="A1:M137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
@@ -8885,10 +8851,10 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="132" t="s">
         <v>157</v>
       </c>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="135" t="s">
         <v>213</v>
       </c>
       <c r="C2" s="17" t="s">
@@ -8920,8 +8886,8 @@
       <c r="M2" s="72"/>
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="108"/>
-      <c r="B3" s="111"/>
+      <c r="A3" s="133"/>
+      <c r="B3" s="136"/>
       <c r="C3" s="32" t="s">
         <v>159</v>
       </c>
@@ -8951,8 +8917,8 @@
       <c r="M3" s="79"/>
     </row>
     <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="108"/>
-      <c r="B4" s="111"/>
+      <c r="A4" s="133"/>
+      <c r="B4" s="136"/>
       <c r="C4" s="23" t="s">
         <v>164</v>
       </c>
@@ -8982,8 +8948,8 @@
       <c r="M4" s="77"/>
     </row>
     <row r="5" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="108"/>
-      <c r="B5" s="111"/>
+      <c r="A5" s="133"/>
+      <c r="B5" s="136"/>
       <c r="C5" s="32" t="s">
         <v>165</v>
       </c>
@@ -9015,8 +8981,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="108"/>
-      <c r="B6" s="111"/>
+      <c r="A6" s="133"/>
+      <c r="B6" s="136"/>
       <c r="C6" s="23" t="s">
         <v>166</v>
       </c>
@@ -9046,8 +9012,8 @@
       <c r="M6" s="77"/>
     </row>
     <row r="7" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="108"/>
-      <c r="B7" s="111"/>
+      <c r="A7" s="133"/>
+      <c r="B7" s="136"/>
       <c r="C7" s="32" t="s">
         <v>171</v>
       </c>
@@ -9079,8 +9045,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="108"/>
-      <c r="B8" s="111"/>
+      <c r="A8" s="133"/>
+      <c r="B8" s="136"/>
       <c r="C8" s="23" t="s">
         <v>172</v>
       </c>
@@ -9110,8 +9076,8 @@
       <c r="M8" s="77"/>
     </row>
     <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="108"/>
-      <c r="B9" s="111"/>
+      <c r="A9" s="133"/>
+      <c r="B9" s="136"/>
       <c r="C9" s="32" t="s">
         <v>176</v>
       </c>
@@ -9141,8 +9107,8 @@
       <c r="M9" s="79"/>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="108"/>
-      <c r="B10" s="111"/>
+      <c r="A10" s="133"/>
+      <c r="B10" s="136"/>
       <c r="C10" s="23" t="s">
         <v>177</v>
       </c>
@@ -9174,8 +9140,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="108"/>
-      <c r="B11" s="111"/>
+      <c r="A11" s="133"/>
+      <c r="B11" s="136"/>
       <c r="C11" s="32" t="s">
         <v>178</v>
       </c>
@@ -9205,8 +9171,8 @@
       <c r="M11" s="79"/>
     </row>
     <row r="12" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="108"/>
-      <c r="B12" s="111"/>
+      <c r="A12" s="133"/>
+      <c r="B12" s="136"/>
       <c r="C12" s="23" t="s">
         <v>179</v>
       </c>
@@ -9236,8 +9202,8 @@
       <c r="M12" s="77"/>
     </row>
     <row r="13" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="108"/>
-      <c r="B13" s="111"/>
+      <c r="A13" s="133"/>
+      <c r="B13" s="136"/>
       <c r="C13" s="32" t="s">
         <v>187</v>
       </c>
@@ -9267,8 +9233,8 @@
       <c r="M13" s="79"/>
     </row>
     <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="108"/>
-      <c r="B14" s="111"/>
+      <c r="A14" s="133"/>
+      <c r="B14" s="136"/>
       <c r="C14" s="23" t="s">
         <v>188</v>
       </c>
@@ -9300,8 +9266,8 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="108"/>
-      <c r="B15" s="111"/>
+      <c r="A15" s="133"/>
+      <c r="B15" s="136"/>
       <c r="C15" s="32" t="s">
         <v>189</v>
       </c>
@@ -9333,8 +9299,8 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="108"/>
-      <c r="B16" s="111"/>
+      <c r="A16" s="133"/>
+      <c r="B16" s="136"/>
       <c r="C16" s="23" t="s">
         <v>190</v>
       </c>
@@ -9364,8 +9330,8 @@
       <c r="M16" s="77"/>
     </row>
     <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="108"/>
-      <c r="B17" s="111"/>
+      <c r="A17" s="133"/>
+      <c r="B17" s="136"/>
       <c r="C17" s="32" t="s">
         <v>200</v>
       </c>
@@ -9395,8 +9361,8 @@
       <c r="M17" s="79"/>
     </row>
     <row r="18" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="108"/>
-      <c r="B18" s="111"/>
+      <c r="A18" s="133"/>
+      <c r="B18" s="136"/>
       <c r="C18" s="23" t="s">
         <v>241</v>
       </c>
@@ -9426,8 +9392,8 @@
       <c r="M18" s="77"/>
     </row>
     <row r="19" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="109"/>
-      <c r="B19" s="112"/>
+      <c r="A19" s="134"/>
+      <c r="B19" s="137"/>
       <c r="C19" s="32" t="s">
         <v>242</v>
       </c>
@@ -9457,10 +9423,10 @@
       <c r="M19" s="79"/>
     </row>
     <row r="20" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="113" t="s">
+      <c r="A20" s="138" t="s">
         <v>210</v>
       </c>
-      <c r="B20" s="96" t="s">
+      <c r="B20" s="123" t="s">
         <v>212</v>
       </c>
       <c r="C20" s="47" t="s">
@@ -9494,8 +9460,8 @@
       <c r="M20" s="74"/>
     </row>
     <row r="21" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="117"/>
-      <c r="B21" s="97"/>
+      <c r="A21" s="139"/>
+      <c r="B21" s="124"/>
       <c r="C21" s="47" t="s">
         <v>215</v>
       </c>
@@ -9525,8 +9491,8 @@
       <c r="M21" s="74"/>
     </row>
     <row r="22" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A22" s="117"/>
-      <c r="B22" s="97"/>
+      <c r="A22" s="139"/>
+      <c r="B22" s="124"/>
       <c r="C22" s="47" t="s">
         <v>216</v>
       </c>
@@ -9556,8 +9522,8 @@
       <c r="M22" s="74"/>
     </row>
     <row r="23" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="117"/>
-      <c r="B23" s="97"/>
+      <c r="A23" s="139"/>
+      <c r="B23" s="124"/>
       <c r="C23" s="47" t="s">
         <v>217</v>
       </c>
@@ -9587,8 +9553,8 @@
       <c r="M23" s="74"/>
     </row>
     <row r="24" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="117"/>
-      <c r="B24" s="97"/>
+      <c r="A24" s="139"/>
+      <c r="B24" s="124"/>
       <c r="C24" s="47" t="s">
         <v>218</v>
       </c>
@@ -9618,8 +9584,8 @@
       <c r="M24" s="74"/>
     </row>
     <row r="25" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="117"/>
-      <c r="B25" s="97"/>
+      <c r="A25" s="139"/>
+      <c r="B25" s="124"/>
       <c r="C25" s="47" t="s">
         <v>219</v>
       </c>
@@ -9649,8 +9615,8 @@
       <c r="M25" s="74"/>
     </row>
     <row r="26" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="117"/>
-      <c r="B26" s="97"/>
+      <c r="A26" s="139"/>
+      <c r="B26" s="124"/>
       <c r="C26" s="47" t="s">
         <v>220</v>
       </c>
@@ -9680,8 +9646,8 @@
       <c r="M26" s="74"/>
     </row>
     <row r="27" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="117"/>
-      <c r="B27" s="97"/>
+      <c r="A27" s="139"/>
+      <c r="B27" s="124"/>
       <c r="C27" s="47" t="s">
         <v>221</v>
       </c>
@@ -9711,8 +9677,8 @@
       <c r="M27" s="74"/>
     </row>
     <row r="28" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="117"/>
-      <c r="B28" s="97"/>
+      <c r="A28" s="139"/>
+      <c r="B28" s="124"/>
       <c r="C28" s="47" t="s">
         <v>222</v>
       </c>
@@ -9742,8 +9708,8 @@
       <c r="M28" s="74"/>
     </row>
     <row r="29" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="117"/>
-      <c r="B29" s="97"/>
+      <c r="A29" s="139"/>
+      <c r="B29" s="124"/>
       <c r="C29" s="47" t="s">
         <v>223</v>
       </c>
@@ -9773,8 +9739,8 @@
       <c r="M29" s="74"/>
     </row>
     <row r="30" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="117"/>
-      <c r="B30" s="97"/>
+      <c r="A30" s="139"/>
+      <c r="B30" s="124"/>
       <c r="C30" s="47" t="s">
         <v>224</v>
       </c>
@@ -9804,8 +9770,8 @@
       <c r="M30" s="74"/>
     </row>
     <row r="31" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="117"/>
-      <c r="B31" s="97"/>
+      <c r="A31" s="139"/>
+      <c r="B31" s="124"/>
       <c r="C31" s="47" t="s">
         <v>225</v>
       </c>
@@ -9835,8 +9801,8 @@
       <c r="M31" s="74"/>
     </row>
     <row r="32" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="117"/>
-      <c r="B32" s="97"/>
+      <c r="A32" s="139"/>
+      <c r="B32" s="124"/>
       <c r="C32" s="47" t="s">
         <v>226</v>
       </c>
@@ -9866,8 +9832,8 @@
       <c r="M32" s="74"/>
     </row>
     <row r="33" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="117"/>
-      <c r="B33" s="97"/>
+      <c r="A33" s="139"/>
+      <c r="B33" s="124"/>
       <c r="C33" s="47" t="s">
         <v>227</v>
       </c>
@@ -9899,8 +9865,8 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="117"/>
-      <c r="B34" s="97"/>
+      <c r="A34" s="139"/>
+      <c r="B34" s="124"/>
       <c r="C34" s="47" t="s">
         <v>228</v>
       </c>
@@ -9930,8 +9896,8 @@
       <c r="M34" s="74"/>
     </row>
     <row r="35" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="117"/>
-      <c r="B35" s="97"/>
+      <c r="A35" s="139"/>
+      <c r="B35" s="124"/>
       <c r="C35" s="47" t="s">
         <v>229</v>
       </c>
@@ -9961,8 +9927,8 @@
       <c r="M35" s="74"/>
     </row>
     <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="117"/>
-      <c r="B36" s="97"/>
+      <c r="A36" s="139"/>
+      <c r="B36" s="124"/>
       <c r="C36" s="47" t="s">
         <v>230</v>
       </c>
@@ -9992,8 +9958,8 @@
       <c r="M36" s="74"/>
     </row>
     <row r="37" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="117"/>
-      <c r="B37" s="97"/>
+      <c r="A37" s="139"/>
+      <c r="B37" s="124"/>
       <c r="C37" s="47" t="s">
         <v>231</v>
       </c>
@@ -10025,8 +9991,8 @@
       </c>
     </row>
     <row r="38" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="117"/>
-      <c r="B38" s="97"/>
+      <c r="A38" s="139"/>
+      <c r="B38" s="124"/>
       <c r="C38" s="47" t="s">
         <v>232</v>
       </c>
@@ -10058,8 +10024,8 @@
       </c>
     </row>
     <row r="39" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="117"/>
-      <c r="B39" s="97"/>
+      <c r="A39" s="139"/>
+      <c r="B39" s="124"/>
       <c r="C39" s="47" t="s">
         <v>233</v>
       </c>
@@ -10089,8 +10055,8 @@
       <c r="M39" s="74"/>
     </row>
     <row r="40" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A40" s="117"/>
-      <c r="B40" s="97"/>
+      <c r="A40" s="139"/>
+      <c r="B40" s="124"/>
       <c r="C40" s="47" t="s">
         <v>234</v>
       </c>
@@ -10120,8 +10086,8 @@
       <c r="M40" s="74"/>
     </row>
     <row r="41" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="117"/>
-      <c r="B41" s="97"/>
+      <c r="A41" s="139"/>
+      <c r="B41" s="124"/>
       <c r="C41" s="47" t="s">
         <v>249</v>
       </c>
@@ -10151,8 +10117,8 @@
       <c r="M41" s="74"/>
     </row>
     <row r="42" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="117"/>
-      <c r="B42" s="97"/>
+      <c r="A42" s="139"/>
+      <c r="B42" s="124"/>
       <c r="C42" s="47" t="s">
         <v>250</v>
       </c>
@@ -10182,8 +10148,8 @@
       <c r="M42" s="74"/>
     </row>
     <row r="43" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="117"/>
-      <c r="B43" s="97"/>
+      <c r="A43" s="139"/>
+      <c r="B43" s="124"/>
       <c r="C43" s="47" t="s">
         <v>251</v>
       </c>
@@ -10213,8 +10179,8 @@
       <c r="M43" s="74"/>
     </row>
     <row r="44" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="117"/>
-      <c r="B44" s="97"/>
+      <c r="A44" s="139"/>
+      <c r="B44" s="124"/>
       <c r="C44" s="47" t="s">
         <v>252</v>
       </c>
@@ -10244,8 +10210,8 @@
       <c r="M44" s="74"/>
     </row>
     <row r="45" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="117"/>
-      <c r="B45" s="97"/>
+      <c r="A45" s="139"/>
+      <c r="B45" s="124"/>
       <c r="C45" s="47" t="s">
         <v>253</v>
       </c>
@@ -10275,8 +10241,8 @@
       <c r="M45" s="74"/>
     </row>
     <row r="46" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="117"/>
-      <c r="B46" s="97"/>
+      <c r="A46" s="139"/>
+      <c r="B46" s="124"/>
       <c r="C46" s="47" t="s">
         <v>254</v>
       </c>
@@ -10306,8 +10272,8 @@
       <c r="M46" s="74"/>
     </row>
     <row r="47" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="117"/>
-      <c r="B47" s="97"/>
+      <c r="A47" s="139"/>
+      <c r="B47" s="124"/>
       <c r="C47" s="47" t="s">
         <v>255</v>
       </c>
@@ -10337,8 +10303,8 @@
       <c r="M47" s="74"/>
     </row>
     <row r="48" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="117"/>
-      <c r="B48" s="97"/>
+      <c r="A48" s="139"/>
+      <c r="B48" s="124"/>
       <c r="C48" s="47" t="s">
         <v>256</v>
       </c>
@@ -10368,8 +10334,8 @@
       <c r="M48" s="74"/>
     </row>
     <row r="49" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" s="117"/>
-      <c r="B49" s="97"/>
+      <c r="A49" s="139"/>
+      <c r="B49" s="124"/>
       <c r="C49" s="47" t="s">
         <v>257</v>
       </c>
@@ -10401,8 +10367,8 @@
       </c>
     </row>
     <row r="50" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="117"/>
-      <c r="B50" s="97"/>
+      <c r="A50" s="139"/>
+      <c r="B50" s="124"/>
       <c r="C50" s="47" t="s">
         <v>258</v>
       </c>
@@ -10432,8 +10398,8 @@
       <c r="M50" s="74"/>
     </row>
     <row r="51" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="117"/>
-      <c r="B51" s="97"/>
+      <c r="A51" s="139"/>
+      <c r="B51" s="124"/>
       <c r="C51" s="47" t="s">
         <v>260</v>
       </c>
@@ -10463,8 +10429,8 @@
       <c r="M51" s="74"/>
     </row>
     <row r="52" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="117"/>
-      <c r="B52" s="97"/>
+      <c r="A52" s="139"/>
+      <c r="B52" s="124"/>
       <c r="C52" s="47" t="s">
         <v>261</v>
       </c>
@@ -10494,8 +10460,8 @@
       <c r="M52" s="74"/>
     </row>
     <row r="53" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A53" s="118"/>
-      <c r="B53" s="98"/>
+      <c r="A53" s="140"/>
+      <c r="B53" s="126"/>
       <c r="C53" s="47" t="s">
         <v>262</v>
       </c>
@@ -10527,10 +10493,10 @@
       </c>
     </row>
     <row r="54" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A54" s="107" t="s">
+      <c r="A54" s="141" t="s">
         <v>639</v>
       </c>
-      <c r="B54" s="110" t="s">
+      <c r="B54" s="142" t="s">
         <v>640</v>
       </c>
       <c r="C54" s="24" t="s">
@@ -10562,8 +10528,8 @@
       <c r="M54" s="77"/>
     </row>
     <row r="55" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A55" s="108"/>
-      <c r="B55" s="111"/>
+      <c r="A55" s="133"/>
+      <c r="B55" s="136"/>
       <c r="C55" s="34" t="s">
         <v>666</v>
       </c>
@@ -10593,8 +10559,8 @@
       <c r="M55" s="79"/>
     </row>
     <row r="56" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="108"/>
-      <c r="B56" s="111"/>
+      <c r="A56" s="133"/>
+      <c r="B56" s="136"/>
       <c r="C56" s="24" t="s">
         <v>667</v>
       </c>
@@ -10624,8 +10590,8 @@
       <c r="M56" s="77"/>
     </row>
     <row r="57" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="108"/>
-      <c r="B57" s="111"/>
+      <c r="A57" s="133"/>
+      <c r="B57" s="136"/>
       <c r="C57" s="34" t="s">
         <v>668</v>
       </c>
@@ -10657,8 +10623,8 @@
       </c>
     </row>
     <row r="58" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="108"/>
-      <c r="B58" s="111"/>
+      <c r="A58" s="133"/>
+      <c r="B58" s="136"/>
       <c r="C58" s="24" t="s">
         <v>669</v>
       </c>
@@ -10690,8 +10656,8 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="108"/>
-      <c r="B59" s="111"/>
+      <c r="A59" s="133"/>
+      <c r="B59" s="136"/>
       <c r="C59" s="34" t="s">
         <v>670</v>
       </c>
@@ -10721,8 +10687,8 @@
       <c r="M59" s="79"/>
     </row>
     <row r="60" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="108"/>
-      <c r="B60" s="111"/>
+      <c r="A60" s="133"/>
+      <c r="B60" s="136"/>
       <c r="C60" s="24" t="s">
         <v>671</v>
       </c>
@@ -10752,8 +10718,8 @@
       <c r="M60" s="77"/>
     </row>
     <row r="61" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="108"/>
-      <c r="B61" s="111"/>
+      <c r="A61" s="133"/>
+      <c r="B61" s="136"/>
       <c r="C61" s="34" t="s">
         <v>672</v>
       </c>
@@ -10783,8 +10749,8 @@
       <c r="M61" s="79"/>
     </row>
     <row r="62" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A62" s="108"/>
-      <c r="B62" s="111"/>
+      <c r="A62" s="133"/>
+      <c r="B62" s="136"/>
       <c r="C62" s="24" t="s">
         <v>673</v>
       </c>
@@ -10814,8 +10780,8 @@
       <c r="M62" s="77"/>
     </row>
     <row r="63" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A63" s="108"/>
-      <c r="B63" s="111"/>
+      <c r="A63" s="133"/>
+      <c r="B63" s="136"/>
       <c r="C63" s="34" t="s">
         <v>674</v>
       </c>
@@ -10845,8 +10811,8 @@
       <c r="M63" s="79"/>
     </row>
     <row r="64" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="109"/>
-      <c r="B64" s="112"/>
+      <c r="A64" s="134"/>
+      <c r="B64" s="137"/>
       <c r="C64" s="24" t="s">
         <v>675</v>
       </c>
@@ -10876,10 +10842,10 @@
       <c r="M64" s="77"/>
     </row>
     <row r="65" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="113" t="s">
+      <c r="A65" s="138" t="s">
         <v>647</v>
       </c>
-      <c r="B65" s="96" t="s">
+      <c r="B65" s="123" t="s">
         <v>641</v>
       </c>
       <c r="C65" s="47" t="s">
@@ -10915,8 +10881,8 @@
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A66" s="117"/>
-      <c r="B66" s="97"/>
+      <c r="A66" s="139"/>
+      <c r="B66" s="124"/>
       <c r="C66" s="47" t="s">
         <v>697</v>
       </c>
@@ -10946,8 +10912,8 @@
       <c r="M66" s="74"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A67" s="118"/>
-      <c r="B67" s="98"/>
+      <c r="A67" s="140"/>
+      <c r="B67" s="126"/>
       <c r="C67" s="47" t="s">
         <v>698</v>
       </c>
@@ -10979,10 +10945,10 @@
       </c>
     </row>
     <row r="68" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="107" t="s">
+      <c r="A68" s="141" t="s">
         <v>648</v>
       </c>
-      <c r="B68" s="110" t="s">
+      <c r="B68" s="142" t="s">
         <v>642</v>
       </c>
       <c r="C68" s="24" t="s">
@@ -11014,8 +10980,8 @@
       <c r="M68" s="77"/>
     </row>
     <row r="69" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A69" s="108"/>
-      <c r="B69" s="111"/>
+      <c r="A69" s="133"/>
+      <c r="B69" s="136"/>
       <c r="C69" s="34" t="s">
         <v>707</v>
       </c>
@@ -11047,8 +11013,8 @@
       </c>
     </row>
     <row r="70" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="108"/>
-      <c r="B70" s="111"/>
+      <c r="A70" s="133"/>
+      <c r="B70" s="136"/>
       <c r="C70" s="24" t="s">
         <v>708</v>
       </c>
@@ -11078,8 +11044,8 @@
       <c r="M70" s="77"/>
     </row>
     <row r="71" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="108"/>
-      <c r="B71" s="111"/>
+      <c r="A71" s="133"/>
+      <c r="B71" s="136"/>
       <c r="C71" s="34" t="s">
         <v>709</v>
       </c>
@@ -11109,8 +11075,8 @@
       <c r="M71" s="79"/>
     </row>
     <row r="72" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="108"/>
-      <c r="B72" s="111"/>
+      <c r="A72" s="133"/>
+      <c r="B72" s="136"/>
       <c r="C72" s="24" t="s">
         <v>710</v>
       </c>
@@ -11142,8 +11108,8 @@
       </c>
     </row>
     <row r="73" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="108"/>
-      <c r="B73" s="111"/>
+      <c r="A73" s="133"/>
+      <c r="B73" s="136"/>
       <c r="C73" s="34" t="s">
         <v>711</v>
       </c>
@@ -11173,8 +11139,8 @@
       <c r="M73" s="79"/>
     </row>
     <row r="74" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="109"/>
-      <c r="B74" s="112"/>
+      <c r="A74" s="134"/>
+      <c r="B74" s="137"/>
       <c r="C74" s="24" t="s">
         <v>712</v>
       </c>
@@ -11204,10 +11170,10 @@
       <c r="M74" s="77"/>
     </row>
     <row r="75" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="113" t="s">
+      <c r="A75" s="138" t="s">
         <v>649</v>
       </c>
-      <c r="B75" s="96" t="s">
+      <c r="B75" s="123" t="s">
         <v>643</v>
       </c>
       <c r="C75" s="47" t="s">
@@ -11241,8 +11207,8 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A76" s="117"/>
-      <c r="B76" s="97"/>
+      <c r="A76" s="139"/>
+      <c r="B76" s="124"/>
       <c r="C76" s="47" t="s">
         <v>713</v>
       </c>
@@ -11272,8 +11238,8 @@
       <c r="M76" s="74"/>
     </row>
     <row r="77" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="118"/>
-      <c r="B77" s="98"/>
+      <c r="A77" s="140"/>
+      <c r="B77" s="126"/>
       <c r="C77" s="47" t="s">
         <v>714</v>
       </c>
@@ -11305,10 +11271,10 @@
       </c>
     </row>
     <row r="78" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" s="107" t="s">
+      <c r="A78" s="141" t="s">
         <v>650</v>
       </c>
-      <c r="B78" s="110" t="s">
+      <c r="B78" s="142" t="s">
         <v>644</v>
       </c>
       <c r="C78" s="24" t="s">
@@ -11342,8 +11308,8 @@
       <c r="M78" s="77"/>
     </row>
     <row r="79" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A79" s="108"/>
-      <c r="B79" s="111"/>
+      <c r="A79" s="133"/>
+      <c r="B79" s="136"/>
       <c r="C79" s="34" t="s">
         <v>733</v>
       </c>
@@ -11373,8 +11339,8 @@
       <c r="M79" s="79"/>
     </row>
     <row r="80" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A80" s="108"/>
-      <c r="B80" s="111"/>
+      <c r="A80" s="133"/>
+      <c r="B80" s="136"/>
       <c r="C80" s="24" t="s">
         <v>734</v>
       </c>
@@ -11404,8 +11370,8 @@
       <c r="M80" s="77"/>
     </row>
     <row r="81" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A81" s="108"/>
-      <c r="B81" s="111"/>
+      <c r="A81" s="133"/>
+      <c r="B81" s="136"/>
       <c r="C81" s="34" t="s">
         <v>735</v>
       </c>
@@ -11435,8 +11401,8 @@
       <c r="M81" s="79"/>
     </row>
     <row r="82" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A82" s="108"/>
-      <c r="B82" s="111"/>
+      <c r="A82" s="133"/>
+      <c r="B82" s="136"/>
       <c r="C82" s="24" t="s">
         <v>736</v>
       </c>
@@ -11466,8 +11432,8 @@
       <c r="M82" s="77"/>
     </row>
     <row r="83" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A83" s="108"/>
-      <c r="B83" s="111"/>
+      <c r="A83" s="133"/>
+      <c r="B83" s="136"/>
       <c r="C83" s="34" t="s">
         <v>737</v>
       </c>
@@ -11499,8 +11465,8 @@
       <c r="M83" s="79"/>
     </row>
     <row r="84" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A84" s="108"/>
-      <c r="B84" s="111"/>
+      <c r="A84" s="133"/>
+      <c r="B84" s="136"/>
       <c r="C84" s="24" t="s">
         <v>738</v>
       </c>
@@ -11530,8 +11496,8 @@
       <c r="M84" s="77"/>
     </row>
     <row r="85" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A85" s="108"/>
-      <c r="B85" s="111"/>
+      <c r="A85" s="133"/>
+      <c r="B85" s="136"/>
       <c r="C85" s="34" t="s">
         <v>739</v>
       </c>
@@ -11561,8 +11527,8 @@
       <c r="M85" s="79"/>
     </row>
     <row r="86" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A86" s="108"/>
-      <c r="B86" s="111"/>
+      <c r="A86" s="133"/>
+      <c r="B86" s="136"/>
       <c r="C86" s="24" t="s">
         <v>740</v>
       </c>
@@ -11592,8 +11558,8 @@
       <c r="M86" s="77"/>
     </row>
     <row r="87" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A87" s="108"/>
-      <c r="B87" s="111"/>
+      <c r="A87" s="133"/>
+      <c r="B87" s="136"/>
       <c r="C87" s="34" t="s">
         <v>741</v>
       </c>
@@ -11623,8 +11589,8 @@
       <c r="M87" s="79"/>
     </row>
     <row r="88" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A88" s="108"/>
-      <c r="B88" s="111"/>
+      <c r="A88" s="133"/>
+      <c r="B88" s="136"/>
       <c r="C88" s="24" t="s">
         <v>742</v>
       </c>
@@ -11654,8 +11620,8 @@
       <c r="M88" s="77"/>
     </row>
     <row r="89" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A89" s="108"/>
-      <c r="B89" s="111"/>
+      <c r="A89" s="133"/>
+      <c r="B89" s="136"/>
       <c r="C89" s="34" t="s">
         <v>743</v>
       </c>
@@ -11685,8 +11651,8 @@
       <c r="M89" s="79"/>
     </row>
     <row r="90" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A90" s="108"/>
-      <c r="B90" s="111"/>
+      <c r="A90" s="133"/>
+      <c r="B90" s="136"/>
       <c r="C90" s="24" t="s">
         <v>744</v>
       </c>
@@ -11716,8 +11682,8 @@
       <c r="M90" s="77"/>
     </row>
     <row r="91" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="108"/>
-      <c r="B91" s="111"/>
+      <c r="A91" s="133"/>
+      <c r="B91" s="136"/>
       <c r="C91" s="34" t="s">
         <v>745</v>
       </c>
@@ -11747,8 +11713,8 @@
       <c r="M91" s="79"/>
     </row>
     <row r="92" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A92" s="108"/>
-      <c r="B92" s="111"/>
+      <c r="A92" s="133"/>
+      <c r="B92" s="136"/>
       <c r="C92" s="24" t="s">
         <v>746</v>
       </c>
@@ -11778,8 +11744,8 @@
       <c r="M92" s="77"/>
     </row>
     <row r="93" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A93" s="108"/>
-      <c r="B93" s="111"/>
+      <c r="A93" s="133"/>
+      <c r="B93" s="136"/>
       <c r="C93" s="34" t="s">
         <v>747</v>
       </c>
@@ -11809,8 +11775,8 @@
       <c r="M93" s="79"/>
     </row>
     <row r="94" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A94" s="108"/>
-      <c r="B94" s="111"/>
+      <c r="A94" s="133"/>
+      <c r="B94" s="136"/>
       <c r="C94" s="24" t="s">
         <v>748</v>
       </c>
@@ -11840,8 +11806,8 @@
       <c r="M94" s="77"/>
     </row>
     <row r="95" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A95" s="108"/>
-      <c r="B95" s="111"/>
+      <c r="A95" s="133"/>
+      <c r="B95" s="136"/>
       <c r="C95" s="34" t="s">
         <v>749</v>
       </c>
@@ -11871,8 +11837,8 @@
       <c r="M95" s="79"/>
     </row>
     <row r="96" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A96" s="108"/>
-      <c r="B96" s="111"/>
+      <c r="A96" s="133"/>
+      <c r="B96" s="136"/>
       <c r="C96" s="24" t="s">
         <v>750</v>
       </c>
@@ -11902,8 +11868,8 @@
       <c r="M96" s="77"/>
     </row>
     <row r="97" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A97" s="108"/>
-      <c r="B97" s="111"/>
+      <c r="A97" s="133"/>
+      <c r="B97" s="136"/>
       <c r="C97" s="34" t="s">
         <v>751</v>
       </c>
@@ -11933,8 +11899,8 @@
       <c r="M97" s="79"/>
     </row>
     <row r="98" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A98" s="109"/>
-      <c r="B98" s="112"/>
+      <c r="A98" s="134"/>
+      <c r="B98" s="137"/>
       <c r="C98" s="24" t="s">
         <v>752</v>
       </c>
@@ -11964,10 +11930,10 @@
       <c r="M98" s="77"/>
     </row>
     <row r="99" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="113" t="s">
+      <c r="A99" s="138" t="s">
         <v>651</v>
       </c>
-      <c r="B99" s="96" t="s">
+      <c r="B99" s="123" t="s">
         <v>645</v>
       </c>
       <c r="C99" s="47" t="s">
@@ -12003,8 +11969,8 @@
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A100" s="117"/>
-      <c r="B100" s="97"/>
+      <c r="A100" s="139"/>
+      <c r="B100" s="124"/>
       <c r="C100" s="47" t="s">
         <v>753</v>
       </c>
@@ -12034,8 +12000,8 @@
       <c r="M100" s="74"/>
     </row>
     <row r="101" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="118"/>
-      <c r="B101" s="98"/>
+      <c r="A101" s="140"/>
+      <c r="B101" s="126"/>
       <c r="C101" s="47" t="s">
         <v>754</v>
       </c>
@@ -12067,10 +12033,10 @@
       </c>
     </row>
     <row r="102" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="107" t="s">
+      <c r="A102" s="141" t="s">
         <v>652</v>
       </c>
-      <c r="B102" s="110" t="s">
+      <c r="B102" s="142" t="s">
         <v>646</v>
       </c>
       <c r="C102" s="24" t="s">
@@ -12106,8 +12072,8 @@
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A103" s="108"/>
-      <c r="B103" s="111"/>
+      <c r="A103" s="133"/>
+      <c r="B103" s="136"/>
       <c r="C103" s="34" t="s">
         <v>755</v>
       </c>
@@ -12137,8 +12103,8 @@
       <c r="M103" s="79"/>
     </row>
     <row r="104" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="109"/>
-      <c r="B104" s="112"/>
+      <c r="A104" s="134"/>
+      <c r="B104" s="137"/>
       <c r="C104" s="24" t="s">
         <v>756</v>
       </c>
@@ -12170,10 +12136,10 @@
       </c>
     </row>
     <row r="105" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A105" s="113" t="s">
+      <c r="A105" s="138" t="s">
         <v>793</v>
       </c>
-      <c r="B105" s="96" t="s">
+      <c r="B105" s="123" t="s">
         <v>795</v>
       </c>
       <c r="C105" s="47" t="s">
@@ -12205,8 +12171,8 @@
       <c r="M105" s="74"/>
     </row>
     <row r="106" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A106" s="117"/>
-      <c r="B106" s="97"/>
+      <c r="A106" s="139"/>
+      <c r="B106" s="124"/>
       <c r="C106" s="47" t="s">
         <v>814</v>
       </c>
@@ -12236,8 +12202,8 @@
       <c r="M106" s="74"/>
     </row>
     <row r="107" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A107" s="117"/>
-      <c r="B107" s="97"/>
+      <c r="A107" s="139"/>
+      <c r="B107" s="124"/>
       <c r="C107" s="47" t="s">
         <v>815</v>
       </c>
@@ -12267,8 +12233,8 @@
       <c r="M107" s="74"/>
     </row>
     <row r="108" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A108" s="117"/>
-      <c r="B108" s="97"/>
+      <c r="A108" s="139"/>
+      <c r="B108" s="124"/>
       <c r="C108" s="47" t="s">
         <v>816</v>
       </c>
@@ -12298,8 +12264,8 @@
       <c r="M108" s="74"/>
     </row>
     <row r="109" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A109" s="117"/>
-      <c r="B109" s="97"/>
+      <c r="A109" s="139"/>
+      <c r="B109" s="124"/>
       <c r="C109" s="47" t="s">
         <v>817</v>
       </c>
@@ -12327,8 +12293,8 @@
       <c r="M109" s="74"/>
     </row>
     <row r="110" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="117"/>
-      <c r="B110" s="97"/>
+      <c r="A110" s="139"/>
+      <c r="B110" s="124"/>
       <c r="C110" s="47" t="s">
         <v>818</v>
       </c>
@@ -12356,8 +12322,8 @@
       <c r="M110" s="74"/>
     </row>
     <row r="111" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="117"/>
-      <c r="B111" s="97"/>
+      <c r="A111" s="139"/>
+      <c r="B111" s="124"/>
       <c r="C111" s="47" t="s">
         <v>819</v>
       </c>
@@ -12385,8 +12351,8 @@
       <c r="M111" s="74"/>
     </row>
     <row r="112" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A112" s="118"/>
-      <c r="B112" s="98"/>
+      <c r="A112" s="140"/>
+      <c r="B112" s="126"/>
       <c r="C112" s="47" t="s">
         <v>820</v>
       </c>
@@ -12414,10 +12380,10 @@
       <c r="M112" s="74"/>
     </row>
     <row r="113" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="105" t="s">
+      <c r="A113" s="143" t="s">
         <v>794</v>
       </c>
-      <c r="B113" s="100" t="s">
+      <c r="B113" s="117" t="s">
         <v>797</v>
       </c>
       <c r="C113" s="34" t="s">
@@ -12447,8 +12413,8 @@
       <c r="M113" s="79"/>
     </row>
     <row r="114" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A114" s="106"/>
-      <c r="B114" s="92"/>
+      <c r="A114" s="144"/>
+      <c r="B114" s="119"/>
       <c r="C114" s="24" t="s">
         <v>807</v>
       </c>
@@ -12476,10 +12442,10 @@
       <c r="M114" s="77"/>
     </row>
     <row r="115" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A115" s="113" t="s">
+      <c r="A115" s="138" t="s">
         <v>796</v>
       </c>
-      <c r="B115" s="96" t="s">
+      <c r="B115" s="123" t="s">
         <v>798</v>
       </c>
       <c r="C115" s="47" t="s">
@@ -12513,8 +12479,8 @@
       <c r="M115" s="74"/>
     </row>
     <row r="116" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A116" s="117"/>
-      <c r="B116" s="97"/>
+      <c r="A116" s="139"/>
+      <c r="B116" s="124"/>
       <c r="C116" s="47" t="s">
         <v>808</v>
       </c>
@@ -12546,8 +12512,8 @@
       <c r="M116" s="74"/>
     </row>
     <row r="117" spans="1:13" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="114"/>
-      <c r="B117" s="102"/>
+      <c r="A117" s="145"/>
+      <c r="B117" s="125"/>
       <c r="C117" s="54" t="s">
         <v>809</v>
       </c>
@@ -12878,30 +12844,30 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A105:A112"/>
+    <mergeCell ref="B105:B112"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="A115:A117"/>
+    <mergeCell ref="B115:B117"/>
+    <mergeCell ref="A78:A98"/>
+    <mergeCell ref="B78:B98"/>
+    <mergeCell ref="A99:A101"/>
+    <mergeCell ref="B99:B101"/>
+    <mergeCell ref="A102:A104"/>
+    <mergeCell ref="B102:B104"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="B68:B74"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="B75:B77"/>
     <mergeCell ref="A2:A19"/>
     <mergeCell ref="B2:B19"/>
     <mergeCell ref="A20:A53"/>
     <mergeCell ref="B20:B53"/>
     <mergeCell ref="A54:A64"/>
     <mergeCell ref="B54:B64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="A68:A74"/>
-    <mergeCell ref="B68:B74"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="A78:A98"/>
-    <mergeCell ref="B78:B98"/>
-    <mergeCell ref="A99:A101"/>
-    <mergeCell ref="B99:B101"/>
-    <mergeCell ref="A102:A104"/>
-    <mergeCell ref="B102:B104"/>
-    <mergeCell ref="A105:A112"/>
-    <mergeCell ref="B105:B112"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="A115:A117"/>
-    <mergeCell ref="B115:B117"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="J2:J121 J124">
@@ -12928,20 +12894,20 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" style="15" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="134" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="96" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="120" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="88" customWidth="1"/>
     <col min="9" max="9" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="137" t="s">
+      <c r="B1" s="98" t="s">
         <v>30</v>
       </c>
       <c r="C1" s="68" t="s">
@@ -12959,7 +12925,7 @@
       <c r="G1" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="121" t="s">
+      <c r="H1" s="89" t="s">
         <v>874</v>
       </c>
       <c r="I1" s="71" t="s">
@@ -12967,1158 +12933,1158 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="158" t="s">
         <v>835</v>
       </c>
-      <c r="B2" s="138" t="s">
+      <c r="B2" s="159" t="s">
         <v>844</v>
       </c>
-      <c r="C2" s="122" t="s">
+      <c r="C2" s="90" t="s">
         <v>836</v>
       </c>
-      <c r="D2" s="122"/>
-      <c r="E2" s="145" t="s">
+      <c r="D2" s="90"/>
+      <c r="E2" s="101" t="s">
         <v>929</v>
       </c>
-      <c r="F2" s="143" t="s">
+      <c r="F2" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="122"/>
-      <c r="H2" s="123">
+      <c r="G2" s="90"/>
+      <c r="H2" s="91">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I2" s="124"/>
+      <c r="I2" s="92"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="129"/>
-      <c r="B3" s="139"/>
-      <c r="C3" s="146" t="s">
+      <c r="A3" s="153"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="102" t="s">
         <v>861</v>
       </c>
-      <c r="D3" s="146"/>
-      <c r="E3" s="145" t="s">
+      <c r="D3" s="102"/>
+      <c r="E3" s="101" t="s">
         <v>930</v>
       </c>
-      <c r="F3" s="147" t="s">
+      <c r="F3" s="103" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="146"/>
-      <c r="H3" s="148">
+      <c r="G3" s="102"/>
+      <c r="H3" s="104">
         <v>3.1E-2</v>
       </c>
-      <c r="I3" s="149"/>
+      <c r="I3" s="105"/>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="129"/>
-      <c r="B4" s="139"/>
-      <c r="C4" s="125" t="s">
+      <c r="A4" s="153"/>
+      <c r="B4" s="160"/>
+      <c r="C4" s="93" t="s">
         <v>862</v>
       </c>
-      <c r="D4" s="125"/>
-      <c r="E4" s="145" t="s">
+      <c r="D4" s="93"/>
+      <c r="E4" s="101" t="s">
         <v>931</v>
       </c>
-      <c r="F4" s="144" t="s">
+      <c r="F4" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="125"/>
-      <c r="H4" s="126">
+      <c r="G4" s="93"/>
+      <c r="H4" s="94">
         <v>1.6E-2</v>
       </c>
-      <c r="I4" s="127"/>
+      <c r="I4" s="95"/>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="129"/>
-      <c r="B5" s="139"/>
-      <c r="C5" s="146" t="s">
+      <c r="A5" s="153"/>
+      <c r="B5" s="160"/>
+      <c r="C5" s="102" t="s">
         <v>863</v>
       </c>
-      <c r="D5" s="146"/>
-      <c r="E5" s="145" t="s">
+      <c r="D5" s="102"/>
+      <c r="E5" s="101" t="s">
         <v>932</v>
       </c>
-      <c r="F5" s="147" t="s">
+      <c r="F5" s="103" t="s">
         <v>91</v>
       </c>
-      <c r="G5" s="146"/>
-      <c r="H5" s="148">
+      <c r="G5" s="102"/>
+      <c r="H5" s="104">
         <v>0</v>
       </c>
-      <c r="I5" s="149"/>
+      <c r="I5" s="105"/>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="130"/>
-      <c r="B6" s="140"/>
-      <c r="C6" s="125" t="s">
+      <c r="A6" s="154"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="93" t="s">
         <v>864</v>
       </c>
-      <c r="D6" s="125"/>
-      <c r="E6" s="145" t="s">
+      <c r="D6" s="93"/>
+      <c r="E6" s="101" t="s">
         <v>933</v>
       </c>
-      <c r="F6" s="144" t="s">
+      <c r="F6" s="100" t="s">
         <v>91</v>
       </c>
-      <c r="G6" s="125"/>
-      <c r="H6" s="126">
+      <c r="G6" s="93"/>
+      <c r="H6" s="94">
         <v>1.6E-2</v>
       </c>
-      <c r="I6" s="127"/>
+      <c r="I6" s="95"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="161" t="s">
+      <c r="A7" s="120" t="s">
         <v>837</v>
       </c>
-      <c r="B7" s="162" t="s">
+      <c r="B7" s="149" t="s">
         <v>845</v>
       </c>
-      <c r="C7" s="163" t="s">
+      <c r="C7" s="109" t="s">
         <v>865</v>
       </c>
-      <c r="D7" s="163"/>
-      <c r="E7" s="171" t="s">
+      <c r="D7" s="109"/>
+      <c r="E7" s="113" t="s">
         <v>934</v>
       </c>
-      <c r="F7" s="163" t="s">
+      <c r="F7" s="109" t="s">
         <v>879</v>
       </c>
-      <c r="G7" s="163"/>
-      <c r="H7" s="164">
+      <c r="G7" s="109"/>
+      <c r="H7" s="110">
         <v>1.6E-2</v>
       </c>
-      <c r="I7" s="165"/>
+      <c r="I7" s="111"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="166"/>
-      <c r="B8" s="167"/>
-      <c r="C8" s="163" t="s">
+      <c r="A8" s="121"/>
+      <c r="B8" s="150"/>
+      <c r="C8" s="109" t="s">
         <v>866</v>
       </c>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163" t="s">
+      <c r="D8" s="109"/>
+      <c r="E8" s="109" t="s">
         <v>935</v>
       </c>
-      <c r="F8" s="163" t="s">
+      <c r="F8" s="109" t="s">
         <v>870</v>
       </c>
-      <c r="G8" s="163"/>
-      <c r="H8" s="164">
+      <c r="G8" s="109"/>
+      <c r="H8" s="110">
         <v>3.1E-2</v>
       </c>
-      <c r="I8" s="165"/>
+      <c r="I8" s="111"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="166"/>
-      <c r="B9" s="167"/>
-      <c r="C9" s="163" t="s">
+      <c r="A9" s="121"/>
+      <c r="B9" s="150"/>
+      <c r="C9" s="109" t="s">
         <v>867</v>
       </c>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163" t="s">
+      <c r="D9" s="109"/>
+      <c r="E9" s="109" t="s">
         <v>936</v>
       </c>
-      <c r="F9" s="163" t="s">
+      <c r="F9" s="109" t="s">
         <v>870</v>
       </c>
-      <c r="G9" s="163"/>
-      <c r="H9" s="164">
+      <c r="G9" s="109"/>
+      <c r="H9" s="110">
         <v>1.6E-2</v>
       </c>
-      <c r="I9" s="165"/>
+      <c r="I9" s="111"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="166"/>
-      <c r="B10" s="167"/>
-      <c r="C10" s="163" t="s">
+      <c r="A10" s="121"/>
+      <c r="B10" s="150"/>
+      <c r="C10" s="109" t="s">
         <v>868</v>
       </c>
-      <c r="D10" s="163"/>
-      <c r="E10" s="163" t="s">
+      <c r="D10" s="109"/>
+      <c r="E10" s="109" t="s">
         <v>937</v>
       </c>
-      <c r="F10" s="163" t="s">
+      <c r="F10" s="109" t="s">
         <v>870</v>
       </c>
-      <c r="G10" s="163"/>
-      <c r="H10" s="164">
+      <c r="G10" s="109"/>
+      <c r="H10" s="110">
         <v>3.1E-2</v>
       </c>
-      <c r="I10" s="165"/>
+      <c r="I10" s="111"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="168"/>
-      <c r="B11" s="169"/>
-      <c r="C11" s="163" t="s">
+      <c r="A11" s="127"/>
+      <c r="B11" s="151"/>
+      <c r="C11" s="109" t="s">
         <v>869</v>
       </c>
-      <c r="D11" s="163"/>
-      <c r="E11" s="163" t="s">
+      <c r="D11" s="109"/>
+      <c r="E11" s="109" t="s">
         <v>938</v>
       </c>
-      <c r="F11" s="163" t="s">
+      <c r="F11" s="109" t="s">
         <v>870</v>
       </c>
-      <c r="G11" s="163"/>
-      <c r="H11" s="164">
+      <c r="G11" s="109"/>
+      <c r="H11" s="110">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I11" s="165"/>
+      <c r="I11" s="111"/>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="136" t="s">
+      <c r="A12" s="23" t="s">
         <v>838</v>
       </c>
-      <c r="B12" s="133" t="s">
+      <c r="B12" s="25" t="s">
         <v>846</v>
       </c>
-      <c r="C12" s="125" t="s">
+      <c r="C12" s="93" t="s">
         <v>881</v>
       </c>
-      <c r="D12" s="125"/>
-      <c r="E12" s="125" t="s">
+      <c r="D12" s="93"/>
+      <c r="E12" s="93" t="s">
         <v>880</v>
       </c>
-      <c r="F12" s="125" t="s">
+      <c r="F12" s="93" t="s">
         <v>492</v>
       </c>
-      <c r="G12" s="125"/>
-      <c r="H12" s="126">
+      <c r="G12" s="93"/>
+      <c r="H12" s="94">
         <v>4.5375E-4</v>
       </c>
-      <c r="I12" s="127"/>
+      <c r="I12" s="95"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="161" t="s">
+      <c r="A13" s="120" t="s">
         <v>839</v>
       </c>
-      <c r="B13" s="162" t="s">
+      <c r="B13" s="149" t="s">
         <v>878</v>
       </c>
-      <c r="C13" s="163" t="s">
+      <c r="C13" s="109" t="s">
         <v>882</v>
       </c>
-      <c r="D13" s="163"/>
-      <c r="E13" s="163" t="s">
+      <c r="D13" s="109"/>
+      <c r="E13" s="109" t="s">
         <v>939</v>
       </c>
-      <c r="F13" s="163" t="s">
+      <c r="F13" s="109" t="s">
         <v>871</v>
       </c>
-      <c r="G13" s="163"/>
-      <c r="H13" s="164">
+      <c r="G13" s="109"/>
+      <c r="H13" s="110">
         <v>0</v>
       </c>
-      <c r="I13" s="165"/>
+      <c r="I13" s="111"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="166"/>
-      <c r="B14" s="167"/>
-      <c r="C14" s="163" t="s">
+      <c r="A14" s="121"/>
+      <c r="B14" s="150"/>
+      <c r="C14" s="109" t="s">
         <v>885</v>
       </c>
-      <c r="D14" s="163"/>
-      <c r="E14" s="163" t="s">
+      <c r="D14" s="109"/>
+      <c r="E14" s="109" t="s">
         <v>940</v>
       </c>
-      <c r="F14" s="163" t="s">
+      <c r="F14" s="109" t="s">
         <v>871</v>
       </c>
-      <c r="G14" s="163"/>
-      <c r="H14" s="164">
+      <c r="G14" s="109"/>
+      <c r="H14" s="110">
         <v>0</v>
       </c>
-      <c r="I14" s="165"/>
+      <c r="I14" s="111"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="166"/>
-      <c r="B15" s="167"/>
-      <c r="C15" s="163" t="s">
+      <c r="A15" s="121"/>
+      <c r="B15" s="150"/>
+      <c r="C15" s="109" t="s">
         <v>886</v>
       </c>
-      <c r="D15" s="163"/>
-      <c r="E15" s="163" t="s">
+      <c r="D15" s="109"/>
+      <c r="E15" s="109" t="s">
         <v>941</v>
       </c>
-      <c r="F15" s="163" t="s">
+      <c r="F15" s="109" t="s">
         <v>871</v>
       </c>
-      <c r="G15" s="163"/>
-      <c r="H15" s="164">
+      <c r="G15" s="109"/>
+      <c r="H15" s="110">
         <v>0</v>
       </c>
-      <c r="I15" s="165"/>
+      <c r="I15" s="111"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="166"/>
-      <c r="B16" s="167"/>
-      <c r="C16" s="163" t="s">
+      <c r="A16" s="121"/>
+      <c r="B16" s="150"/>
+      <c r="C16" s="109" t="s">
         <v>887</v>
       </c>
-      <c r="D16" s="163"/>
-      <c r="E16" s="163" t="s">
+      <c r="D16" s="109"/>
+      <c r="E16" s="109" t="s">
         <v>942</v>
       </c>
-      <c r="F16" s="163" t="s">
+      <c r="F16" s="109" t="s">
         <v>871</v>
       </c>
-      <c r="G16" s="163"/>
-      <c r="H16" s="164">
+      <c r="G16" s="109"/>
+      <c r="H16" s="110">
         <v>0</v>
       </c>
-      <c r="I16" s="165"/>
+      <c r="I16" s="111"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="168"/>
-      <c r="B17" s="169"/>
-      <c r="C17" s="163" t="s">
+      <c r="A17" s="127"/>
+      <c r="B17" s="151"/>
+      <c r="C17" s="109" t="s">
         <v>888</v>
       </c>
-      <c r="D17" s="163"/>
-      <c r="E17" s="163" t="s">
+      <c r="D17" s="109"/>
+      <c r="E17" s="109" t="s">
         <v>943</v>
       </c>
-      <c r="F17" s="163" t="s">
+      <c r="F17" s="109" t="s">
         <v>871</v>
       </c>
-      <c r="G17" s="163"/>
-      <c r="H17" s="164">
+      <c r="G17" s="109"/>
+      <c r="H17" s="110">
         <v>0</v>
       </c>
-      <c r="I17" s="165"/>
+      <c r="I17" s="111"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="141" t="s">
+      <c r="A18" s="152" t="s">
         <v>840</v>
       </c>
-      <c r="B18" s="142" t="s">
+      <c r="B18" s="155" t="s">
         <v>847</v>
       </c>
-      <c r="C18" s="125" t="s">
+      <c r="C18" s="93" t="s">
         <v>883</v>
       </c>
-      <c r="D18" s="125"/>
-      <c r="E18" s="125" t="s">
+      <c r="D18" s="93"/>
+      <c r="E18" s="93" t="s">
         <v>939</v>
       </c>
-      <c r="F18" s="125" t="s">
+      <c r="F18" s="93" t="s">
         <v>875</v>
       </c>
-      <c r="G18" s="125"/>
-      <c r="H18" s="126">
+      <c r="G18" s="93"/>
+      <c r="H18" s="94">
         <v>0</v>
       </c>
-      <c r="I18" s="127"/>
+      <c r="I18" s="95"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="129"/>
-      <c r="B19" s="131"/>
-      <c r="C19" s="146" t="s">
+      <c r="A19" s="153"/>
+      <c r="B19" s="156"/>
+      <c r="C19" s="102" t="s">
         <v>925</v>
       </c>
-      <c r="D19" s="146"/>
-      <c r="E19" s="125" t="s">
+      <c r="D19" s="102"/>
+      <c r="E19" s="93" t="s">
         <v>940</v>
       </c>
-      <c r="F19" s="146" t="s">
+      <c r="F19" s="102" t="s">
         <v>875</v>
       </c>
-      <c r="G19" s="146"/>
-      <c r="H19" s="148">
+      <c r="G19" s="102"/>
+      <c r="H19" s="104">
         <v>0</v>
       </c>
-      <c r="I19" s="149"/>
+      <c r="I19" s="105"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="129"/>
-      <c r="B20" s="131"/>
-      <c r="C20" s="125" t="s">
+      <c r="A20" s="153"/>
+      <c r="B20" s="156"/>
+      <c r="C20" s="93" t="s">
         <v>926</v>
       </c>
-      <c r="D20" s="125"/>
-      <c r="E20" s="125" t="s">
+      <c r="D20" s="93"/>
+      <c r="E20" s="93" t="s">
         <v>941</v>
       </c>
-      <c r="F20" s="125" t="s">
+      <c r="F20" s="93" t="s">
         <v>875</v>
       </c>
-      <c r="G20" s="125"/>
-      <c r="H20" s="126">
+      <c r="G20" s="93"/>
+      <c r="H20" s="94">
         <v>0</v>
       </c>
-      <c r="I20" s="127"/>
+      <c r="I20" s="95"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="129"/>
-      <c r="B21" s="131"/>
-      <c r="C21" s="146" t="s">
+      <c r="A21" s="153"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="102" t="s">
         <v>927</v>
       </c>
-      <c r="D21" s="146"/>
-      <c r="E21" s="125" t="s">
+      <c r="D21" s="102"/>
+      <c r="E21" s="93" t="s">
         <v>942</v>
       </c>
-      <c r="F21" s="146" t="s">
+      <c r="F21" s="102" t="s">
         <v>875</v>
       </c>
-      <c r="G21" s="146"/>
-      <c r="H21" s="148">
+      <c r="G21" s="102"/>
+      <c r="H21" s="104">
         <v>0</v>
       </c>
-      <c r="I21" s="149"/>
+      <c r="I21" s="105"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="130"/>
-      <c r="B22" s="132"/>
-      <c r="C22" s="125" t="s">
+      <c r="A22" s="154"/>
+      <c r="B22" s="157"/>
+      <c r="C22" s="93" t="s">
         <v>928</v>
       </c>
-      <c r="D22" s="125"/>
-      <c r="E22" s="125" t="s">
+      <c r="D22" s="93"/>
+      <c r="E22" s="93" t="s">
         <v>943</v>
       </c>
-      <c r="F22" s="125" t="s">
+      <c r="F22" s="93" t="s">
         <v>875</v>
       </c>
-      <c r="G22" s="125"/>
-      <c r="H22" s="126">
+      <c r="G22" s="93"/>
+      <c r="H22" s="94">
         <v>0</v>
       </c>
-      <c r="I22" s="127"/>
+      <c r="I22" s="95"/>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="161" t="s">
+      <c r="A23" s="120" t="s">
         <v>841</v>
       </c>
-      <c r="B23" s="162" t="s">
+      <c r="B23" s="149" t="s">
         <v>848</v>
       </c>
-      <c r="C23" s="163" t="s">
+      <c r="C23" s="109" t="s">
         <v>884</v>
       </c>
-      <c r="D23" s="163"/>
-      <c r="E23" s="170" t="s">
+      <c r="D23" s="109"/>
+      <c r="E23" s="112" t="s">
         <v>929</v>
       </c>
-      <c r="F23" s="163" t="s">
+      <c r="F23" s="109" t="s">
         <v>872</v>
       </c>
-      <c r="G23" s="163"/>
-      <c r="H23" s="164">
+      <c r="G23" s="109"/>
+      <c r="H23" s="110">
         <v>0</v>
       </c>
-      <c r="I23" s="165"/>
+      <c r="I23" s="111"/>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="166"/>
-      <c r="B24" s="167"/>
-      <c r="C24" s="163" t="s">
+      <c r="A24" s="121"/>
+      <c r="B24" s="150"/>
+      <c r="C24" s="109" t="s">
         <v>916</v>
       </c>
-      <c r="D24" s="163"/>
-      <c r="E24" s="170" t="s">
+      <c r="D24" s="109"/>
+      <c r="E24" s="112" t="s">
         <v>930</v>
       </c>
-      <c r="F24" s="163" t="s">
+      <c r="F24" s="109" t="s">
         <v>872</v>
       </c>
-      <c r="G24" s="163"/>
-      <c r="H24" s="164">
+      <c r="G24" s="109"/>
+      <c r="H24" s="110">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="I24" s="165"/>
+      <c r="I24" s="111"/>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="166"/>
-      <c r="B25" s="167"/>
-      <c r="C25" s="163" t="s">
+      <c r="A25" s="121"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="109" t="s">
         <v>917</v>
       </c>
-      <c r="D25" s="163"/>
-      <c r="E25" s="170" t="s">
+      <c r="D25" s="109"/>
+      <c r="E25" s="112" t="s">
         <v>931</v>
       </c>
-      <c r="F25" s="163" t="s">
+      <c r="F25" s="109" t="s">
         <v>872</v>
       </c>
-      <c r="G25" s="163"/>
-      <c r="H25" s="164">
+      <c r="G25" s="109"/>
+      <c r="H25" s="110">
         <v>1.6E-2</v>
       </c>
-      <c r="I25" s="165"/>
+      <c r="I25" s="111"/>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="166"/>
-      <c r="B26" s="167"/>
-      <c r="C26" s="163" t="s">
+      <c r="A26" s="121"/>
+      <c r="B26" s="150"/>
+      <c r="C26" s="109" t="s">
         <v>918</v>
       </c>
-      <c r="D26" s="163"/>
-      <c r="E26" s="170" t="s">
+      <c r="D26" s="109"/>
+      <c r="E26" s="112" t="s">
         <v>932</v>
       </c>
-      <c r="F26" s="163" t="s">
+      <c r="F26" s="109" t="s">
         <v>872</v>
       </c>
-      <c r="G26" s="163"/>
-      <c r="H26" s="164">
+      <c r="G26" s="109"/>
+      <c r="H26" s="110">
         <v>0</v>
       </c>
-      <c r="I26" s="165"/>
+      <c r="I26" s="111"/>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="166"/>
-      <c r="B27" s="167"/>
-      <c r="C27" s="163" t="s">
+      <c r="A27" s="121"/>
+      <c r="B27" s="150"/>
+      <c r="C27" s="109" t="s">
         <v>919</v>
       </c>
-      <c r="D27" s="163"/>
-      <c r="E27" s="170" t="s">
+      <c r="D27" s="109"/>
+      <c r="E27" s="112" t="s">
         <v>933</v>
       </c>
-      <c r="F27" s="163" t="s">
+      <c r="F27" s="109" t="s">
         <v>872</v>
       </c>
-      <c r="G27" s="163"/>
-      <c r="H27" s="164">
+      <c r="G27" s="109"/>
+      <c r="H27" s="110">
         <v>1.6E-2</v>
       </c>
-      <c r="I27" s="165"/>
+      <c r="I27" s="111"/>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="166"/>
-      <c r="B28" s="167"/>
-      <c r="C28" s="163" t="s">
+      <c r="A28" s="121"/>
+      <c r="B28" s="150"/>
+      <c r="C28" s="109" t="s">
         <v>920</v>
       </c>
-      <c r="D28" s="163"/>
-      <c r="E28" s="170" t="s">
+      <c r="D28" s="109"/>
+      <c r="E28" s="112" t="s">
         <v>944</v>
       </c>
-      <c r="F28" s="163" t="s">
+      <c r="F28" s="109" t="s">
         <v>876</v>
       </c>
-      <c r="G28" s="163"/>
-      <c r="H28" s="164">
+      <c r="G28" s="109"/>
+      <c r="H28" s="110">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I28" s="165"/>
+      <c r="I28" s="111"/>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="166"/>
-      <c r="B29" s="167"/>
-      <c r="C29" s="163" t="s">
+      <c r="A29" s="121"/>
+      <c r="B29" s="150"/>
+      <c r="C29" s="109" t="s">
         <v>921</v>
       </c>
-      <c r="D29" s="163"/>
-      <c r="E29" s="170" t="s">
+      <c r="D29" s="109"/>
+      <c r="E29" s="112" t="s">
         <v>945</v>
       </c>
-      <c r="F29" s="163" t="s">
+      <c r="F29" s="109" t="s">
         <v>876</v>
       </c>
-      <c r="G29" s="163"/>
-      <c r="H29" s="164">
+      <c r="G29" s="109"/>
+      <c r="H29" s="110">
         <v>1.6E-2</v>
       </c>
-      <c r="I29" s="165"/>
+      <c r="I29" s="111"/>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="166"/>
-      <c r="B30" s="167"/>
-      <c r="C30" s="163" t="s">
+      <c r="A30" s="121"/>
+      <c r="B30" s="150"/>
+      <c r="C30" s="109" t="s">
         <v>922</v>
       </c>
-      <c r="D30" s="163"/>
-      <c r="E30" s="170" t="s">
+      <c r="D30" s="109"/>
+      <c r="E30" s="112" t="s">
         <v>946</v>
       </c>
-      <c r="F30" s="163" t="s">
+      <c r="F30" s="109" t="s">
         <v>876</v>
       </c>
-      <c r="G30" s="163"/>
-      <c r="H30" s="164">
+      <c r="G30" s="109"/>
+      <c r="H30" s="110">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="I30" s="165"/>
+      <c r="I30" s="111"/>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="166"/>
-      <c r="B31" s="167"/>
-      <c r="C31" s="163" t="s">
+      <c r="A31" s="121"/>
+      <c r="B31" s="150"/>
+      <c r="C31" s="109" t="s">
         <v>923</v>
       </c>
-      <c r="D31" s="163"/>
-      <c r="E31" s="170" t="s">
+      <c r="D31" s="109"/>
+      <c r="E31" s="112" t="s">
         <v>947</v>
       </c>
-      <c r="F31" s="163" t="s">
+      <c r="F31" s="109" t="s">
         <v>876</v>
       </c>
-      <c r="G31" s="163"/>
-      <c r="H31" s="164">
+      <c r="G31" s="109"/>
+      <c r="H31" s="110">
         <v>1.6E-2</v>
       </c>
-      <c r="I31" s="165"/>
+      <c r="I31" s="111"/>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="168"/>
-      <c r="B32" s="169"/>
-      <c r="C32" s="163" t="s">
+      <c r="A32" s="127"/>
+      <c r="B32" s="151"/>
+      <c r="C32" s="109" t="s">
         <v>924</v>
       </c>
-      <c r="D32" s="163"/>
-      <c r="E32" s="170" t="s">
+      <c r="D32" s="109"/>
+      <c r="E32" s="112" t="s">
         <v>948</v>
       </c>
-      <c r="F32" s="163" t="s">
+      <c r="F32" s="109" t="s">
         <v>876</v>
       </c>
-      <c r="G32" s="163"/>
-      <c r="H32" s="164">
+      <c r="G32" s="109"/>
+      <c r="H32" s="110">
         <v>3.1E-2</v>
       </c>
-      <c r="I32" s="165"/>
+      <c r="I32" s="111"/>
     </row>
     <row r="33" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="150" t="s">
+      <c r="A33" s="114" t="s">
         <v>842</v>
       </c>
-      <c r="B33" s="151" t="s">
+      <c r="B33" s="146" t="s">
         <v>849</v>
       </c>
-      <c r="C33" s="146" t="s">
+      <c r="C33" s="102" t="s">
         <v>889</v>
       </c>
-      <c r="D33" s="146"/>
-      <c r="E33" s="146" t="s">
+      <c r="D33" s="102"/>
+      <c r="E33" s="102" t="s">
         <v>939</v>
       </c>
-      <c r="F33" s="146" t="s">
+      <c r="F33" s="102" t="s">
         <v>873</v>
       </c>
-      <c r="G33" s="146"/>
-      <c r="H33" s="148">
+      <c r="G33" s="102"/>
+      <c r="H33" s="104">
         <v>0</v>
       </c>
-      <c r="I33" s="149"/>
+      <c r="I33" s="105"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="152"/>
-      <c r="B34" s="153"/>
-      <c r="C34" s="125" t="s">
+      <c r="A34" s="115"/>
+      <c r="B34" s="147"/>
+      <c r="C34" s="93" t="s">
         <v>912</v>
       </c>
-      <c r="D34" s="125"/>
-      <c r="E34" s="146" t="s">
+      <c r="D34" s="93"/>
+      <c r="E34" s="102" t="s">
         <v>940</v>
       </c>
-      <c r="F34" s="125" t="s">
+      <c r="F34" s="93" t="s">
         <v>873</v>
       </c>
-      <c r="G34" s="125"/>
-      <c r="H34" s="126">
+      <c r="G34" s="93"/>
+      <c r="H34" s="94">
         <v>0</v>
       </c>
-      <c r="I34" s="127"/>
+      <c r="I34" s="95"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="152"/>
-      <c r="B35" s="153"/>
-      <c r="C35" s="146" t="s">
+      <c r="A35" s="115"/>
+      <c r="B35" s="147"/>
+      <c r="C35" s="102" t="s">
         <v>913</v>
       </c>
-      <c r="D35" s="146"/>
-      <c r="E35" s="146" t="s">
+      <c r="D35" s="102"/>
+      <c r="E35" s="102" t="s">
         <v>941</v>
       </c>
-      <c r="F35" s="146" t="s">
+      <c r="F35" s="102" t="s">
         <v>873</v>
       </c>
-      <c r="G35" s="146"/>
-      <c r="H35" s="148">
+      <c r="G35" s="102"/>
+      <c r="H35" s="104">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I35" s="149"/>
+      <c r="I35" s="105"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="152"/>
-      <c r="B36" s="153"/>
-      <c r="C36" s="125" t="s">
+      <c r="A36" s="115"/>
+      <c r="B36" s="147"/>
+      <c r="C36" s="93" t="s">
         <v>914</v>
       </c>
-      <c r="D36" s="125"/>
-      <c r="E36" s="146" t="s">
+      <c r="D36" s="93"/>
+      <c r="E36" s="102" t="s">
         <v>942</v>
       </c>
-      <c r="F36" s="125" t="s">
+      <c r="F36" s="93" t="s">
         <v>873</v>
       </c>
-      <c r="G36" s="125"/>
-      <c r="H36" s="126">
+      <c r="G36" s="93"/>
+      <c r="H36" s="94">
         <v>0</v>
       </c>
-      <c r="I36" s="127"/>
+      <c r="I36" s="95"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="154"/>
-      <c r="B37" s="155"/>
-      <c r="C37" s="146" t="s">
+      <c r="A37" s="116"/>
+      <c r="B37" s="148"/>
+      <c r="C37" s="102" t="s">
         <v>915</v>
       </c>
-      <c r="D37" s="146"/>
-      <c r="E37" s="146" t="s">
+      <c r="D37" s="102"/>
+      <c r="E37" s="102" t="s">
         <v>943</v>
       </c>
-      <c r="F37" s="146" t="s">
+      <c r="F37" s="102" t="s">
         <v>873</v>
       </c>
-      <c r="G37" s="146"/>
-      <c r="H37" s="148">
+      <c r="G37" s="102"/>
+      <c r="H37" s="104">
         <v>0</v>
       </c>
-      <c r="I37" s="149"/>
+      <c r="I37" s="105"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="161" t="s">
+      <c r="A38" s="120" t="s">
         <v>843</v>
       </c>
-      <c r="B38" s="162" t="s">
+      <c r="B38" s="149" t="s">
         <v>850</v>
       </c>
-      <c r="C38" s="163" t="s">
+      <c r="C38" s="109" t="s">
         <v>890</v>
       </c>
-      <c r="D38" s="163"/>
-      <c r="E38" s="163" t="s">
+      <c r="D38" s="109"/>
+      <c r="E38" s="109" t="s">
         <v>939</v>
       </c>
-      <c r="F38" s="163" t="s">
+      <c r="F38" s="109" t="s">
         <v>498</v>
       </c>
-      <c r="G38" s="163"/>
-      <c r="H38" s="164">
+      <c r="G38" s="109"/>
+      <c r="H38" s="110">
         <v>0</v>
       </c>
-      <c r="I38" s="165"/>
+      <c r="I38" s="111"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="166"/>
-      <c r="B39" s="167"/>
-      <c r="C39" s="163" t="s">
+      <c r="A39" s="121"/>
+      <c r="B39" s="150"/>
+      <c r="C39" s="109" t="s">
         <v>908</v>
       </c>
-      <c r="D39" s="163"/>
-      <c r="E39" s="163" t="s">
+      <c r="D39" s="109"/>
+      <c r="E39" s="109" t="s">
         <v>940</v>
       </c>
-      <c r="F39" s="163" t="s">
+      <c r="F39" s="109" t="s">
         <v>498</v>
       </c>
-      <c r="G39" s="163"/>
-      <c r="H39" s="164">
+      <c r="G39" s="109"/>
+      <c r="H39" s="110">
         <v>0</v>
       </c>
-      <c r="I39" s="165"/>
+      <c r="I39" s="111"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="166"/>
-      <c r="B40" s="167"/>
-      <c r="C40" s="163" t="s">
+      <c r="A40" s="121"/>
+      <c r="B40" s="150"/>
+      <c r="C40" s="109" t="s">
         <v>909</v>
       </c>
-      <c r="D40" s="163"/>
-      <c r="E40" s="163" t="s">
+      <c r="D40" s="109"/>
+      <c r="E40" s="109" t="s">
         <v>941</v>
       </c>
-      <c r="F40" s="163" t="s">
+      <c r="F40" s="109" t="s">
         <v>498</v>
       </c>
-      <c r="G40" s="163"/>
-      <c r="H40" s="164">
+      <c r="G40" s="109"/>
+      <c r="H40" s="110">
         <v>1.6E-2</v>
       </c>
-      <c r="I40" s="165"/>
+      <c r="I40" s="111"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="166"/>
-      <c r="B41" s="167"/>
-      <c r="C41" s="163" t="s">
+      <c r="A41" s="121"/>
+      <c r="B41" s="150"/>
+      <c r="C41" s="109" t="s">
         <v>910</v>
       </c>
-      <c r="D41" s="163"/>
-      <c r="E41" s="163" t="s">
+      <c r="D41" s="109"/>
+      <c r="E41" s="109" t="s">
         <v>942</v>
       </c>
-      <c r="F41" s="163" t="s">
+      <c r="F41" s="109" t="s">
         <v>498</v>
       </c>
-      <c r="G41" s="163"/>
-      <c r="H41" s="164">
+      <c r="G41" s="109"/>
+      <c r="H41" s="110">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I41" s="165"/>
+      <c r="I41" s="111"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="168"/>
-      <c r="B42" s="169"/>
-      <c r="C42" s="163" t="s">
+      <c r="A42" s="127"/>
+      <c r="B42" s="151"/>
+      <c r="C42" s="109" t="s">
         <v>911</v>
       </c>
-      <c r="D42" s="163"/>
-      <c r="E42" s="163" t="s">
+      <c r="D42" s="109"/>
+      <c r="E42" s="109" t="s">
         <v>943</v>
       </c>
-      <c r="F42" s="163" t="s">
+      <c r="F42" s="109" t="s">
         <v>498</v>
       </c>
-      <c r="G42" s="163"/>
-      <c r="H42" s="164">
+      <c r="G42" s="109"/>
+      <c r="H42" s="110">
         <v>0</v>
       </c>
-      <c r="I42" s="165"/>
+      <c r="I42" s="111"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="150" t="s">
+      <c r="A43" s="114" t="s">
         <v>851</v>
       </c>
-      <c r="B43" s="151" t="s">
+      <c r="B43" s="146" t="s">
         <v>856</v>
       </c>
-      <c r="C43" s="146" t="s">
+      <c r="C43" s="102" t="s">
         <v>891</v>
       </c>
-      <c r="D43" s="146"/>
-      <c r="E43" s="146" t="s">
+      <c r="D43" s="102"/>
+      <c r="E43" s="102" t="s">
         <v>939</v>
       </c>
-      <c r="F43" s="146" t="s">
+      <c r="F43" s="102" t="s">
         <v>511</v>
       </c>
-      <c r="G43" s="146"/>
-      <c r="H43" s="148">
+      <c r="G43" s="102"/>
+      <c r="H43" s="104">
         <v>0</v>
       </c>
-      <c r="I43" s="149"/>
+      <c r="I43" s="105"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="152"/>
-      <c r="B44" s="153"/>
-      <c r="C44" s="125" t="s">
+      <c r="A44" s="115"/>
+      <c r="B44" s="147"/>
+      <c r="C44" s="93" t="s">
         <v>904</v>
       </c>
-      <c r="D44" s="125"/>
-      <c r="E44" s="146" t="s">
+      <c r="D44" s="93"/>
+      <c r="E44" s="102" t="s">
         <v>940</v>
       </c>
-      <c r="F44" s="125" t="s">
+      <c r="F44" s="93" t="s">
         <v>511</v>
       </c>
-      <c r="G44" s="125"/>
-      <c r="H44" s="126">
+      <c r="G44" s="93"/>
+      <c r="H44" s="94">
         <v>0</v>
       </c>
-      <c r="I44" s="127"/>
+      <c r="I44" s="95"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="152"/>
-      <c r="B45" s="153"/>
-      <c r="C45" s="146" t="s">
+      <c r="A45" s="115"/>
+      <c r="B45" s="147"/>
+      <c r="C45" s="102" t="s">
         <v>905</v>
       </c>
-      <c r="D45" s="146"/>
-      <c r="E45" s="146" t="s">
+      <c r="D45" s="102"/>
+      <c r="E45" s="102" t="s">
         <v>941</v>
       </c>
-      <c r="F45" s="146" t="s">
+      <c r="F45" s="102" t="s">
         <v>511</v>
       </c>
-      <c r="G45" s="146"/>
-      <c r="H45" s="148">
+      <c r="G45" s="102"/>
+      <c r="H45" s="104">
         <v>1.6E-2</v>
       </c>
-      <c r="I45" s="149"/>
+      <c r="I45" s="105"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="152"/>
-      <c r="B46" s="153"/>
-      <c r="C46" s="125" t="s">
+      <c r="A46" s="115"/>
+      <c r="B46" s="147"/>
+      <c r="C46" s="93" t="s">
         <v>906</v>
       </c>
-      <c r="D46" s="125"/>
-      <c r="E46" s="146" t="s">
+      <c r="D46" s="93"/>
+      <c r="E46" s="102" t="s">
         <v>942</v>
       </c>
-      <c r="F46" s="125" t="s">
+      <c r="F46" s="93" t="s">
         <v>511</v>
       </c>
-      <c r="G46" s="125"/>
-      <c r="H46" s="126">
+      <c r="G46" s="93"/>
+      <c r="H46" s="94">
         <v>0</v>
       </c>
-      <c r="I46" s="127"/>
+      <c r="I46" s="95"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="154"/>
-      <c r="B47" s="155"/>
-      <c r="C47" s="146" t="s">
+      <c r="A47" s="116"/>
+      <c r="B47" s="148"/>
+      <c r="C47" s="102" t="s">
         <v>907</v>
       </c>
-      <c r="D47" s="146"/>
-      <c r="E47" s="146" t="s">
+      <c r="D47" s="102"/>
+      <c r="E47" s="102" t="s">
         <v>943</v>
       </c>
-      <c r="F47" s="146" t="s">
+      <c r="F47" s="102" t="s">
         <v>511</v>
       </c>
-      <c r="G47" s="146"/>
-      <c r="H47" s="148">
+      <c r="G47" s="102"/>
+      <c r="H47" s="104">
         <v>0</v>
       </c>
-      <c r="I47" s="149"/>
+      <c r="I47" s="105"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="161" t="s">
+      <c r="A48" s="120" t="s">
         <v>852</v>
       </c>
-      <c r="B48" s="162" t="s">
+      <c r="B48" s="149" t="s">
         <v>857</v>
       </c>
-      <c r="C48" s="163" t="s">
+      <c r="C48" s="109" t="s">
         <v>892</v>
       </c>
-      <c r="D48" s="163"/>
-      <c r="E48" s="163" t="s">
+      <c r="D48" s="109"/>
+      <c r="E48" s="109" t="s">
         <v>939</v>
       </c>
-      <c r="F48" s="163" t="s">
+      <c r="F48" s="109" t="s">
         <v>517</v>
       </c>
-      <c r="G48" s="163"/>
-      <c r="H48" s="164">
+      <c r="G48" s="109"/>
+      <c r="H48" s="110">
         <v>0</v>
       </c>
-      <c r="I48" s="165"/>
+      <c r="I48" s="111"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="166"/>
-      <c r="B49" s="167"/>
-      <c r="C49" s="163" t="s">
+      <c r="A49" s="121"/>
+      <c r="B49" s="150"/>
+      <c r="C49" s="109" t="s">
         <v>900</v>
       </c>
-      <c r="D49" s="163"/>
-      <c r="E49" s="163" t="s">
+      <c r="D49" s="109"/>
+      <c r="E49" s="109" t="s">
         <v>940</v>
       </c>
-      <c r="F49" s="163" t="s">
+      <c r="F49" s="109" t="s">
         <v>517</v>
       </c>
-      <c r="G49" s="163"/>
-      <c r="H49" s="164">
+      <c r="G49" s="109"/>
+      <c r="H49" s="110">
         <v>0</v>
       </c>
-      <c r="I49" s="165"/>
+      <c r="I49" s="111"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="166"/>
-      <c r="B50" s="167"/>
-      <c r="C50" s="163" t="s">
+      <c r="A50" s="121"/>
+      <c r="B50" s="150"/>
+      <c r="C50" s="109" t="s">
         <v>901</v>
       </c>
-      <c r="D50" s="163"/>
-      <c r="E50" s="163" t="s">
+      <c r="D50" s="109"/>
+      <c r="E50" s="109" t="s">
         <v>941</v>
       </c>
-      <c r="F50" s="163" t="s">
+      <c r="F50" s="109" t="s">
         <v>517</v>
       </c>
-      <c r="G50" s="163"/>
-      <c r="H50" s="164">
+      <c r="G50" s="109"/>
+      <c r="H50" s="110">
         <v>0</v>
       </c>
-      <c r="I50" s="165"/>
+      <c r="I50" s="111"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="166"/>
-      <c r="B51" s="167"/>
-      <c r="C51" s="163" t="s">
+      <c r="A51" s="121"/>
+      <c r="B51" s="150"/>
+      <c r="C51" s="109" t="s">
         <v>902</v>
       </c>
-      <c r="D51" s="163"/>
-      <c r="E51" s="163" t="s">
+      <c r="D51" s="109"/>
+      <c r="E51" s="109" t="s">
         <v>942</v>
       </c>
-      <c r="F51" s="163" t="s">
+      <c r="F51" s="109" t="s">
         <v>517</v>
       </c>
-      <c r="G51" s="163"/>
-      <c r="H51" s="164">
+      <c r="G51" s="109"/>
+      <c r="H51" s="110">
         <v>1.6E-2</v>
       </c>
-      <c r="I51" s="165"/>
+      <c r="I51" s="111"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="168"/>
-      <c r="B52" s="169"/>
-      <c r="C52" s="163" t="s">
+      <c r="A52" s="127"/>
+      <c r="B52" s="151"/>
+      <c r="C52" s="109" t="s">
         <v>903</v>
       </c>
-      <c r="D52" s="163"/>
-      <c r="E52" s="163" t="s">
+      <c r="D52" s="109"/>
+      <c r="E52" s="109" t="s">
         <v>943</v>
       </c>
-      <c r="F52" s="163" t="s">
+      <c r="F52" s="109" t="s">
         <v>517</v>
       </c>
-      <c r="G52" s="163"/>
-      <c r="H52" s="164">
+      <c r="G52" s="109"/>
+      <c r="H52" s="110">
         <v>0</v>
       </c>
-      <c r="I52" s="165"/>
+      <c r="I52" s="111"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="150" t="s">
+      <c r="A53" s="114" t="s">
         <v>853</v>
       </c>
-      <c r="B53" s="151" t="s">
+      <c r="B53" s="146" t="s">
         <v>858</v>
       </c>
-      <c r="C53" s="146" t="s">
+      <c r="C53" s="102" t="s">
         <v>893</v>
       </c>
-      <c r="D53" s="146"/>
-      <c r="E53" s="146" t="s">
+      <c r="D53" s="102"/>
+      <c r="E53" s="102" t="s">
         <v>939</v>
       </c>
-      <c r="F53" s="146" t="s">
+      <c r="F53" s="102" t="s">
         <v>518</v>
       </c>
-      <c r="G53" s="146"/>
-      <c r="H53" s="148">
+      <c r="G53" s="102"/>
+      <c r="H53" s="104">
         <v>0</v>
       </c>
-      <c r="I53" s="149"/>
+      <c r="I53" s="105"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="152"/>
-      <c r="B54" s="153"/>
-      <c r="C54" s="125" t="s">
+      <c r="A54" s="115"/>
+      <c r="B54" s="147"/>
+      <c r="C54" s="93" t="s">
         <v>896</v>
       </c>
-      <c r="D54" s="125"/>
-      <c r="E54" s="146" t="s">
+      <c r="D54" s="93"/>
+      <c r="E54" s="102" t="s">
         <v>940</v>
       </c>
-      <c r="F54" s="125" t="s">
+      <c r="F54" s="93" t="s">
         <v>518</v>
       </c>
-      <c r="G54" s="125"/>
-      <c r="H54" s="126">
+      <c r="G54" s="93"/>
+      <c r="H54" s="94">
         <v>0</v>
       </c>
-      <c r="I54" s="127"/>
+      <c r="I54" s="95"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="152"/>
-      <c r="B55" s="153"/>
-      <c r="C55" s="146" t="s">
+      <c r="A55" s="115"/>
+      <c r="B55" s="147"/>
+      <c r="C55" s="102" t="s">
         <v>897</v>
       </c>
-      <c r="D55" s="146"/>
-      <c r="E55" s="146" t="s">
+      <c r="D55" s="102"/>
+      <c r="E55" s="102" t="s">
         <v>941</v>
       </c>
-      <c r="F55" s="146" t="s">
+      <c r="F55" s="102" t="s">
         <v>518</v>
       </c>
-      <c r="G55" s="146"/>
-      <c r="H55" s="148">
+      <c r="G55" s="102"/>
+      <c r="H55" s="104">
         <v>0</v>
       </c>
-      <c r="I55" s="149"/>
+      <c r="I55" s="105"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="152"/>
-      <c r="B56" s="153"/>
-      <c r="C56" s="125" t="s">
+      <c r="A56" s="115"/>
+      <c r="B56" s="147"/>
+      <c r="C56" s="93" t="s">
         <v>898</v>
       </c>
-      <c r="D56" s="125"/>
-      <c r="E56" s="146" t="s">
+      <c r="D56" s="93"/>
+      <c r="E56" s="102" t="s">
         <v>942</v>
       </c>
-      <c r="F56" s="125" t="s">
+      <c r="F56" s="93" t="s">
         <v>518</v>
       </c>
-      <c r="G56" s="125"/>
-      <c r="H56" s="126">
+      <c r="G56" s="93"/>
+      <c r="H56" s="94">
         <v>0</v>
       </c>
-      <c r="I56" s="127"/>
+      <c r="I56" s="95"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="154"/>
-      <c r="B57" s="155"/>
-      <c r="C57" s="146" t="s">
+      <c r="A57" s="116"/>
+      <c r="B57" s="148"/>
+      <c r="C57" s="102" t="s">
         <v>899</v>
       </c>
-      <c r="D57" s="146"/>
-      <c r="E57" s="146" t="s">
+      <c r="D57" s="102"/>
+      <c r="E57" s="102" t="s">
         <v>943</v>
       </c>
-      <c r="F57" s="146" t="s">
+      <c r="F57" s="102" t="s">
         <v>518</v>
       </c>
-      <c r="G57" s="146"/>
-      <c r="H57" s="148">
+      <c r="G57" s="102"/>
+      <c r="H57" s="104">
         <v>0</v>
       </c>
-      <c r="I57" s="149"/>
+      <c r="I57" s="105"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="172" t="s">
+      <c r="A58" s="30" t="s">
         <v>854</v>
       </c>
-      <c r="B58" s="173" t="s">
+      <c r="B58" s="48" t="s">
         <v>859</v>
       </c>
-      <c r="C58" s="163" t="s">
+      <c r="C58" s="109" t="s">
         <v>894</v>
       </c>
-      <c r="D58" s="163"/>
-      <c r="E58" s="163" t="s">
+      <c r="D58" s="109"/>
+      <c r="E58" s="109" t="s">
         <v>880</v>
       </c>
-      <c r="F58" s="163" t="s">
+      <c r="F58" s="109" t="s">
         <v>525</v>
       </c>
-      <c r="G58" s="163"/>
-      <c r="H58" s="164">
+      <c r="G58" s="109"/>
+      <c r="H58" s="110">
         <v>1.6E-2</v>
       </c>
-      <c r="I58" s="165"/>
+      <c r="I58" s="111"/>
     </row>
     <row r="59" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="156" t="s">
+      <c r="A59" s="41" t="s">
         <v>855</v>
       </c>
-      <c r="B59" s="157" t="s">
+      <c r="B59" s="42" t="s">
         <v>860</v>
       </c>
-      <c r="C59" s="158" t="s">
+      <c r="C59" s="106" t="s">
         <v>895</v>
       </c>
-      <c r="D59" s="158"/>
-      <c r="E59" s="158" t="s">
+      <c r="D59" s="106"/>
+      <c r="E59" s="106" t="s">
         <v>880</v>
       </c>
-      <c r="F59" s="158" t="s">
+      <c r="F59" s="106" t="s">
         <v>877</v>
       </c>
-      <c r="G59" s="158"/>
-      <c r="H59" s="159">
+      <c r="G59" s="106"/>
+      <c r="H59" s="107">
         <v>0</v>
       </c>
-      <c r="I59" s="160"/>
+      <c r="I59" s="108"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="16"/>
@@ -14128,7 +14094,7 @@
       <c r="E60" s="2"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="119"/>
+      <c r="H60" s="87"/>
       <c r="I60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -14139,7 +14105,7 @@
       <c r="E61" s="2"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="H61" s="119"/>
+      <c r="H61" s="87"/>
       <c r="I61" s="2"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -14150,7 +14116,7 @@
       <c r="E62" s="2"/>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="119"/>
+      <c r="H62" s="87"/>
       <c r="I62" s="2"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -14161,7 +14127,7 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="119"/>
+      <c r="H63" s="87"/>
       <c r="I63" s="2"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -14172,7 +14138,7 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="119"/>
+      <c r="H64" s="87"/>
       <c r="I64" s="2"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -14183,7 +14149,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="119"/>
+      <c r="H65" s="87"/>
       <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -14194,7 +14160,7 @@
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="119"/>
+      <c r="H66" s="87"/>
       <c r="I66" s="2"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -14205,7 +14171,7 @@
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="119"/>
+      <c r="H67" s="87"/>
       <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -14216,7 +14182,7 @@
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="119"/>
+      <c r="H68" s="87"/>
       <c r="I68" s="2"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -14227,7 +14193,7 @@
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="119"/>
+      <c r="H69" s="87"/>
       <c r="I69" s="2"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -14238,7 +14204,7 @@
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="119"/>
+      <c r="H70" s="87"/>
       <c r="I70" s="2"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -14249,7 +14215,7 @@
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="119"/>
+      <c r="H71" s="87"/>
       <c r="I71" s="2"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -14260,7 +14226,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="119"/>
+      <c r="H72" s="87"/>
       <c r="I72" s="2"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -14271,7 +14237,7 @@
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
-      <c r="H73" s="119"/>
+      <c r="H73" s="87"/>
       <c r="I73" s="2"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -14282,7 +14248,7 @@
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
-      <c r="H74" s="119"/>
+      <c r="H74" s="87"/>
       <c r="I74" s="2"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -14293,7 +14259,7 @@
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
-      <c r="H75" s="119"/>
+      <c r="H75" s="87"/>
       <c r="I75" s="2"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -14304,7 +14270,7 @@
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="119"/>
+      <c r="H76" s="87"/>
       <c r="I76" s="2"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -14315,7 +14281,7 @@
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-      <c r="H77" s="119"/>
+      <c r="H77" s="87"/>
       <c r="I77" s="2"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -14326,7 +14292,7 @@
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
-      <c r="H78" s="119"/>
+      <c r="H78" s="87"/>
       <c r="I78" s="2"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -14337,7 +14303,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
-      <c r="H79" s="119"/>
+      <c r="H79" s="87"/>
       <c r="I79" s="2"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -14348,7 +14314,7 @@
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="119"/>
+      <c r="H80" s="87"/>
       <c r="I80" s="2"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -14359,11 +14325,23 @@
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
-      <c r="H81" s="119"/>
+      <c r="H81" s="87"/>
       <c r="I81" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="B33:B37"/>
     <mergeCell ref="A53:A57"/>
     <mergeCell ref="B53:B57"/>
     <mergeCell ref="A38:A42"/>
@@ -14372,18 +14350,6 @@
     <mergeCell ref="B43:B47"/>
     <mergeCell ref="A48:A52"/>
     <mergeCell ref="B48:B52"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="B23:B32"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B13:B17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>